<commit_message>
#131: add new storagenode feature to list of supported functionalities.
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evetion/code/HYDROLIB-core/docs/topics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEEB695-A4A8-944E-9BA7-BCE936065D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14E0B8-ED43-41CA-A6C0-24DACCBE3FC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -30,10 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="133">
   <si>
     <t>Functionality</t>
   </si>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
+  </si>
+  <si>
+    <t>Storage node file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.storagenode.models</t>
+  </si>
+  <si>
+    <t>StorageNodeModel</t>
   </si>
 </sst>
 </file>
@@ -799,12 +805,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -824,7 +830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A2)," ",'Source table'!A2)</f>
         <v>**DIMR**</v>
@@ -850,7 +856,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A3)," ",'Source table'!A3)</f>
         <v>`dimr_config.xml`</v>
@@ -876,7 +882,7 @@
         <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A4)," ",'Source table'!A4)</f>
         <v>FM component</v>
@@ -902,7 +908,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A5)," ",'Source table'!A5)</f>
         <v>RR component</v>
@@ -928,7 +934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A6)," ",'Source table'!A6)</f>
         <v>RTC component</v>
@@ -954,7 +960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A7)," ",'Source table'!A7)</f>
         <v>parallel MPI models</v>
@@ -980,7 +986,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A8)," ",'Source table'!A8)</f>
         <v>coupler elements</v>
@@ -1008,27 +1014,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0CF6A0-E039-4E9E-A3D4-429B45288E31}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,158 +1055,132 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
-        <v>0.1.5</v>
-      </c>
-      <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
-      </c>
-      <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
-        <v>Rainfall .bui file</v>
-      </c>
-      <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="D4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v>0.1.5</v>
       </c>
-      <c r="E4" s="3" t="str">
+      <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
-      </c>
-      <c r="F4" s="3" t="str">
+        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
+      </c>
+      <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <v>Rainfall .bui file</v>
+      </c>
+      <c r="B4" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <v>0.1.5</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <v>_Moved to io.rr in 0.1.6_</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
-        <v>0.1.6*</v>
-      </c>
-      <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
-        <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
-      </c>
-      <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
-        <v>Link file 3b_link.tp</v>
-      </c>
-      <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
-      </c>
-      <c r="D7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v>0.1.6*</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E6" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
-        <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
-      </c>
-      <c r="F7" s="3" t="str">
+        <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
+      </c>
+      <c r="F6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -1218,9 +1199,9 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A10)," ",'Source table'!A10)</f>
         <v>**FM**</v>
@@ -1266,7 +1247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A11)," ",'Source table'!A11)</f>
         <v>MDU file</v>
@@ -1292,7 +1273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A12)," ",'Source table'!A12)</f>
         <v>Network file `_net.nc`</v>
@@ -1318,7 +1299,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A13)," ",'Source table'!A13)</f>
         <v>**Structure file**</v>
@@ -1344,7 +1325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A14)," ",'Source table'!A14)</f>
         <v>* Weir</v>
@@ -1370,7 +1351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A15)," ",'Source table'!A15)</f>
         <v>* Universal weir</v>
@@ -1396,7 +1377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A16)," ",'Source table'!A16)</f>
         <v>* Culvert</v>
@@ -1422,7 +1403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A17)," ",'Source table'!A17)</f>
         <v>* Long culvert</v>
@@ -1448,7 +1429,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A18)," ",'Source table'!A18)</f>
         <v>* Bridge</v>
@@ -1474,7 +1455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A19)," ",'Source table'!A19)</f>
         <v>* Pump</v>
@@ -1500,7 +1481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A20)," ",'Source table'!A20)</f>
         <v>* Orifice</v>
@@ -1526,7 +1507,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A21)," ",'Source table'!A21)</f>
         <v>* Gate</v>
@@ -1552,7 +1533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A22)," ",'Source table'!A22)</f>
         <v>* General structure</v>
@@ -1578,7 +1559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A23)," ",'Source table'!A23)</f>
         <v>* Dambreak</v>
@@ -1604,7 +1585,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A24)," ",'Source table'!A24)</f>
         <v>* Compound structure</v>
@@ -1630,7 +1611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A25)," ",'Source table'!A25)</f>
         <v>External forcings file (old)</v>
@@ -1656,7 +1637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A26)," ",'Source table'!A26)</f>
         <v>**External forcings file (new)**</v>
@@ -1682,7 +1663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A27)," ",'Source table'!A27)</f>
         <v>* Boundary</v>
@@ -1708,7 +1689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A28)," ",'Source table'!A28)</f>
         <v>* Lateral</v>
@@ -1734,7 +1715,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A29)," ",'Source table'!A29)</f>
         <v>* Meteo</v>
@@ -1760,7 +1741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A30)," ",'Source table'!A30)</f>
         <v>* .bc file</v>
@@ -1786,7 +1767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
         <v>**Cross section files**</v>
@@ -1812,7 +1793,7 @@
         <v>_Moved to io.crosssections in 0.1.6._</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
         <v>Cross section definition file</v>
@@ -1838,7 +1819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
         <v>* Circle</v>
@@ -1864,7 +1845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
         <v>* Rectangle</v>
@@ -1890,7 +1871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
         <v>* Tabulated river</v>
@@ -1916,7 +1897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
         <v>* ZW (tabulated)</v>
@@ -1942,7 +1923,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
         <v>* XYZ</v>
@@ -1968,7 +1949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>* YZ</v>
@@ -1994,7 +1975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section location file</v>
@@ -2020,7 +2001,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>1D roughness file</v>
@@ -2046,44 +2027,44 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
-        <v>**Output**</v>
+        <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.1.6*</v>
       </c>
       <c r="E33" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
-        <v>Observation station file (old)</v>
+        <v>**Output**</v>
       </c>
       <c r="B34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
@@ -2098,18 +2079,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
-        <v>Observation station file (new)</v>
+        <v>Observation station file (old)</v>
       </c>
       <c r="B35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
@@ -2124,18 +2105,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
-        <v>Observation crosssection file (old)</v>
+        <v>Observation station file (new)</v>
       </c>
       <c r="B36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
@@ -2150,18 +2131,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
-        <v>Observation crosssection file (new)</v>
+        <v>Observation crosssection file (old)</v>
       </c>
       <c r="B37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
@@ -2176,10 +2157,10 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
-        <v>History file `_his.nc`</v>
+        <v>Observation crosssection file (new)</v>
       </c>
       <c r="B38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2202,18 +2183,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
-        <v>Map file (old)</v>
+        <v>History file `_his.nc`</v>
       </c>
       <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
@@ -2228,18 +2209,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
-        <v>Map file (UGRID) `_map.nc`</v>
+        <v>Map file (old)</v>
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
@@ -2254,18 +2235,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
-        <v>Fourier input file</v>
+        <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
@@ -2280,18 +2261,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
-        <v>Fourier output file `_fou.nc`</v>
+        <v>Fourier input file</v>
       </c>
       <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
@@ -2303,13 +2284,13 @@
       </c>
       <c r="F42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
-        <v>_via map file reader_</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
-        <v>Class map file</v>
+        <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2332,18 +2313,18 @@
         <v>_via map file reader_</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
-        <v xml:space="preserve"> </v>
+        <v>Class map file</v>
       </c>
       <c r="B44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
@@ -2355,33 +2336,34 @@
       </c>
       <c r="F44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
-        <v xml:space="preserve"> </v>
+        <v>_via map file reader_</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2404,12 +2386,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2432,7 +2414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2452,7 +2434,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2472,7 +2454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2486,7 +2468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2506,7 +2488,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2526,12 +2508,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2551,7 +2533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2571,7 +2553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2591,7 +2573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2611,7 +2593,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2631,7 +2613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2651,7 +2633,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2662,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2682,7 +2664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2702,7 +2684,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2722,7 +2704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2735,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2773,7 +2755,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2793,7 +2775,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +2786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -2824,7 +2806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2844,7 +2826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2864,7 +2846,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2875,7 +2857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2895,7 +2877,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2909,7 +2891,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2929,7 +2911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2949,7 +2931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -2969,7 +2951,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2989,7 +2971,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -3009,7 +2991,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -3029,7 +3011,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -3049,7 +3031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3069,7 +3051,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -3089,58 +3071,67 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>103</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>11</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>105</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>106</v>
-      </c>
-      <c r="B45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>107</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -3149,56 +3140,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>109</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>110</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>111</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>113</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3210,37 +3198,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>115</v>
-      </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>57</v>
-      </c>
-      <c r="E54" t="s">
-        <v>117</v>
-      </c>
-      <c r="F54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>118</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -3252,43 +3231,46 @@
         <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
+      <c r="E56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" t="s">
+        <v>120</v>
+      </c>
+      <c r="G56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>122</v>
-      </c>
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" t="s">
-        <v>124</v>
-      </c>
-      <c r="F57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -3303,6 +3285,26 @@
         <v>124</v>
       </c>
       <c r="F58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3321,13 +3323,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3371,7 +3373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
#119: Add inifield and onedfield to apidocs and list of supported functionalities.
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evetion/code/HYDROLIB-core/docs/topics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEEB695-A4A8-944E-9BA7-BCE936065D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6841EBB-83FB-4A16-98A8-CD15A73403FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -30,10 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="140">
   <si>
     <t>Functionality</t>
   </si>
@@ -431,6 +428,36 @@
   </si>
   <si>
     <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
+  </si>
+  <si>
+    <t>Initial and parameter field file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.inifield.models</t>
+  </si>
+  <si>
+    <t>IniFieldModel</t>
+  </si>
+  <si>
+    <t>Sample file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.xyz.models</t>
+  </si>
+  <si>
+    <t>XYZModel</t>
+  </si>
+  <si>
+    <t>1D field INI files</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.onedfield.models</t>
+  </si>
+  <si>
+    <t>OneDFieldModel</t>
+  </si>
+  <si>
+    <t>**Spatial data files**</t>
   </si>
 </sst>
 </file>
@@ -799,12 +826,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -824,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A2)," ",'Source table'!A2)</f>
         <v>**DIMR**</v>
@@ -850,7 +881,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A3)," ",'Source table'!A3)</f>
         <v>`dimr_config.xml`</v>
@@ -876,7 +907,7 @@
         <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A4)," ",'Source table'!A4)</f>
         <v>FM component</v>
@@ -902,7 +933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A5)," ",'Source table'!A5)</f>
         <v>RR component</v>
@@ -928,7 +959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A6)," ",'Source table'!A6)</f>
         <v>RTC component</v>
@@ -954,7 +985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A7)," ",'Source table'!A7)</f>
         <v>parallel MPI models</v>
@@ -980,7 +1011,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A8)," ",'Source table'!A8)</f>
         <v>coupler elements</v>
@@ -1008,6 +1039,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1016,19 +1048,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="A3:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1048,159 +1080,159 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v>0.1.6*</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Link file 3b_link.tp</v>
       </c>
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v>0.1.6*</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1212,15 +1244,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A10)," ",'Source table'!A10)</f>
         <v>**FM**</v>
@@ -1266,7 +1304,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A11)," ",'Source table'!A11)</f>
         <v>MDU file</v>
@@ -1292,7 +1330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A12)," ",'Source table'!A12)</f>
         <v>Network file `_net.nc`</v>
@@ -1318,7 +1356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A13)," ",'Source table'!A13)</f>
         <v>**Structure file**</v>
@@ -1344,7 +1382,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A14)," ",'Source table'!A14)</f>
         <v>* Weir</v>
@@ -1370,7 +1408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A15)," ",'Source table'!A15)</f>
         <v>* Universal weir</v>
@@ -1396,7 +1434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A16)," ",'Source table'!A16)</f>
         <v>* Culvert</v>
@@ -1422,7 +1460,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A17)," ",'Source table'!A17)</f>
         <v>* Long culvert</v>
@@ -1448,7 +1486,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A18)," ",'Source table'!A18)</f>
         <v>* Bridge</v>
@@ -1474,7 +1512,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A19)," ",'Source table'!A19)</f>
         <v>* Pump</v>
@@ -1500,7 +1538,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A20)," ",'Source table'!A20)</f>
         <v>* Orifice</v>
@@ -1526,7 +1564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A21)," ",'Source table'!A21)</f>
         <v>* Gate</v>
@@ -1552,7 +1590,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A22)," ",'Source table'!A22)</f>
         <v>* General structure</v>
@@ -1578,7 +1616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A23)," ",'Source table'!A23)</f>
         <v>* Dambreak</v>
@@ -1604,7 +1642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A24)," ",'Source table'!A24)</f>
         <v>* Compound structure</v>
@@ -1630,7 +1668,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A25)," ",'Source table'!A25)</f>
         <v>External forcings file (old)</v>
@@ -1656,7 +1694,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A26)," ",'Source table'!A26)</f>
         <v>**External forcings file (new)**</v>
@@ -1682,7 +1720,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A27)," ",'Source table'!A27)</f>
         <v>* Boundary</v>
@@ -1708,7 +1746,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A28)," ",'Source table'!A28)</f>
         <v>* Lateral</v>
@@ -1734,7 +1772,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A29)," ",'Source table'!A29)</f>
         <v>* Meteo</v>
@@ -1760,7 +1798,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A30)," ",'Source table'!A30)</f>
         <v>* .bc file</v>
@@ -1786,7 +1824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
         <v>**Cross section files**</v>
@@ -1812,7 +1850,7 @@
         <v>_Moved to io.crosssections in 0.1.6._</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
         <v>Cross section definition file</v>
@@ -1838,7 +1876,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
         <v>* Circle</v>
@@ -1864,7 +1902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
         <v>* Rectangle</v>
@@ -1890,7 +1928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
         <v>* Tabulated river</v>
@@ -1916,7 +1954,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
         <v>* ZW (tabulated)</v>
@@ -1942,7 +1980,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
         <v>* XYZ</v>
@@ -1968,7 +2006,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>* YZ</v>
@@ -1994,7 +2032,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section location file</v>
@@ -2020,7 +2058,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>1D roughness file</v>
@@ -2046,10 +2084,10 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
-        <v>**Output**</v>
+        <v>**Spatial data files**</v>
       </c>
       <c r="B33" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2072,96 +2110,96 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
-        <v>Observation station file (old)</v>
+        <v>Initial and parameter field file</v>
       </c>
       <c r="B34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.1.6*</v>
       </c>
       <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
-        <v>Observation station file (new)</v>
+        <v>1D field INI files</v>
       </c>
       <c r="B35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.1.6*</v>
       </c>
       <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
-        <v>Observation crosssection file (old)</v>
+        <v>Sample file</v>
       </c>
       <c r="B36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.1.1</v>
       </c>
       <c r="E36" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
-        <v>Observation crosssection file (new)</v>
+        <v>**Output**</v>
       </c>
       <c r="B37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
@@ -2176,18 +2214,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
-        <v>History file `_his.nc`</v>
+        <v>Observation station file (old)</v>
       </c>
       <c r="B38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
@@ -2202,18 +2240,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
-        <v>Map file (old)</v>
+        <v>Observation station file (new)</v>
       </c>
       <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
@@ -2228,18 +2266,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
-        <v>Map file (UGRID) `_map.nc`</v>
+        <v>Observation crosssection file (old)</v>
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
@@ -2254,18 +2292,18 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
-        <v>Fourier input file</v>
+        <v>Observation crosssection file (new)</v>
       </c>
       <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
@@ -2280,10 +2318,10 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
-        <v>Fourier output file `_fou.nc`</v>
+        <v>History file `_his.nc`</v>
       </c>
       <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2303,21 +2341,21 @@
       </c>
       <c r="F42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
-        <v>_via map file reader_</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
-        <v>Class map file</v>
+        <v>Map file (old)</v>
       </c>
       <c r="B43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="C43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:x:</v>
       </c>
       <c r="D43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
@@ -2329,21 +2367,21 @@
       </c>
       <c r="F43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
-        <v>_via map file reader_</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
-        <v xml:space="preserve"> </v>
+        <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="C44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>:material-close-box:</v>
       </c>
       <c r="D44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
@@ -2358,30 +2396,109 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <v>Fourier input file</v>
+      </c>
+      <c r="B45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="C45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E45" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <v>Fourier output file `_fou.nc`</v>
+      </c>
+      <c r="B46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <v>_via map file reader_</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <v>Class map file</v>
+      </c>
+      <c r="B47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <v>_via map file reader_</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2404,12 +2521,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2432,7 +2549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2452,7 +2569,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2472,7 +2589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2486,7 +2603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2506,7 +2623,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2526,12 +2643,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2551,7 +2668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2571,7 +2688,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2591,7 +2708,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2611,7 +2728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2631,7 +2748,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2651,7 +2768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2662,7 +2779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2682,7 +2799,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2702,7 +2819,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2722,7 +2839,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2870,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2773,7 +2890,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2793,7 +2910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +2921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -2824,7 +2941,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2844,7 +2961,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2864,7 +2981,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2875,7 +2992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2895,7 +3012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2909,7 +3026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2929,7 +3046,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2949,7 +3066,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -2969,7 +3086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -2989,7 +3106,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -3009,7 +3126,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -3029,7 +3146,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -3049,7 +3166,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3069,7 +3186,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -3089,102 +3206,123 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>103</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>105</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>106</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>107</v>
-      </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>111</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3192,117 +3330,161 @@
       <c r="C50" t="s">
         <v>11</v>
       </c>
-      <c r="G50" t="s">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B55" t="s">
         <v>11</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C55" t="s">
         <v>11</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G55" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>115</v>
       </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
         <v>57</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E58" t="s">
         <v>117</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F58" t="s">
         <v>116</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G58" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>118</v>
       </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
         <v>57</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E59" t="s">
         <v>119</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F59" t="s">
         <v>120</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G59" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>122</v>
       </c>
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
         <v>58</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E61" t="s">
         <v>124</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F61" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>125</v>
       </c>
-      <c r="B58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
         <v>58</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E62" t="s">
         <v>124</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F62" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3321,13 +3503,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -3338,7 +3520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3349,7 +3531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -3360,7 +3542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3371,7 +3553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Feature/119 inifield file (#182)
* #119: inifield namespace, IniFieldModel + all enums

* Create inifield.md

* #119: full definition of InitialField and ParameterField + first unit tests.

* #119: missing line

* #119: test for case sensitive parsing of inifield enums.

* #119: validate value+dataFileType polygon

* Comment only

* #119: added forgotten initialFields.ini

* typo in docstring

* #119 Add !1D field INI file format

* #119: Add inifield and onedfield to apidocs and list of supported functionalities.

* #119 Include IniFieldModel in mdu/FMModel

* Create 1dfield.ini

* #119 review comments

* #119: Reduce complexity

* less complex?

* Update util.py

* #119: enabled get_required_fields_validator() for AbstractSpatialField.value

Co-authored-by: Prisca van der Sluis <priscavdsluis@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14E0B8-ED43-41CA-A6C0-24DACCBE3FC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FFE0C-6B07-4B7A-8BB1-43AFDDF35353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="143">
   <si>
     <t>Functionality</t>
   </si>
@@ -428,6 +428,36 @@
   </si>
   <si>
     <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
+  </si>
+  <si>
+    <t>Initial and parameter field file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.inifield.models</t>
+  </si>
+  <si>
+    <t>IniFieldModel</t>
+  </si>
+  <si>
+    <t>Sample file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.xyz.models</t>
+  </si>
+  <si>
+    <t>XYZModel</t>
+  </si>
+  <si>
+    <t>1D field INI files</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.onedfield.models</t>
+  </si>
+  <si>
+    <t>OneDFieldModel</t>
+  </si>
+  <si>
+    <t>**Spatial data files**</t>
   </si>
   <si>
     <t>Storage node file</t>
@@ -807,7 +837,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,16 +1048,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0CF6A0-E039-4E9E-A3D4-429B45288E31}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,131 +1091,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v>_Moved to io.rr in 0.1.6_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v>0.1.6*</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <v>Link file 3b_link.tp</v>
+      </c>
+      <c r="B7" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <v>0.1.6*</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1193,13 +1253,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -2029,328 +2095,406 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
-        <v>Storage node file</v>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <v>**Spatial data files**</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:white_check_mark:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
-        <v>0.1.6*</v>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
-        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
-        <v>**Output**</v>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <v>Initial and parameter field file</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v xml:space="preserve"> </v>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <v>0.1.6*</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
-        <v>Observation station file (old)</v>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <v>1D field INI files</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <v>0.1.6*</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
-        <v>Observation station file (new)</v>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <v>Sample file</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <v>0.1.1</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
-        <v>Observation crosssection file (old)</v>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <v>**Output**</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
-        <v>Observation crosssection file (new)</v>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <v>Observation station file (old)</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
-        <v>History file `_his.nc`</v>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <v>Observation station file (new)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
-        <v>Map file (old)</v>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <v>Observation crosssection file (old)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
-        <v>Map file (UGRID) `_map.nc`</v>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <v>Observation crosssection file (new)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
-        <v>Fourier input file</v>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <v>History file `_his.nc`</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
-        <v>Fourier output file `_fou.nc`</v>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <v>Map file (old)</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
-        <v>_via map file reader_</v>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <v>Map file (UGRID) `_map.nc`</v>
+      </c>
+      <c r="B44" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C44" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E44" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F44" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <v>Fourier input file</v>
+      </c>
+      <c r="B45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="C45" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:x:</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E45" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F45" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <v>Fourier output file `_fou.nc`</v>
+      </c>
+      <c r="B46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="C46" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:material-close-box:</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F46" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <v>_via map file reader_</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Class map file</v>
       </c>
-      <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+      <c r="B47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+      <c r="C47" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E44" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F47" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,7 +3217,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3085,108 +3229,129 @@
         <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3194,122 +3359,166 @@
       <c r="C51" t="s">
         <v>11</v>
       </c>
-      <c r="G51" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E59" t="s">
+        <v>117</v>
+      </c>
+      <c r="F59" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" t="s">
+        <v>124</v>
+      </c>
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>125</v>
       </c>
-      <c r="B59" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
         <v>58</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E63" t="s">
         <v>124</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F63" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G58" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G59" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete 0.2.0 changelog + site consistency
* missing topics/tutorials in nav
* Changelog
* mkdocs-macros for easy linking to GitHub and User Manuals.
* list of funtionalities find/replace 0.1.6* -> 0.2.0
* added HYDROLIB logo (but needs a white version)
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FFE0C-6B07-4B7A-8BB1-43AFDDF35353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DE795-08E2-4835-AD20-F6D8D3171D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>0.1.5</t>
   </si>
   <si>
-    <t>0.1.6*</t>
-  </si>
-  <si>
     <t>UniversalWeir</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Cross section location file</t>
   </si>
   <si>
-    <t>Moved to io.crosssections in 0.1.6.</t>
-  </si>
-  <si>
     <t>hydrolib.core.io.crosssection.models</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
     <t>BuiModel</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.1.6</t>
-  </si>
-  <si>
     <t>Node file 3b_node.tp</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>**RR**</t>
   </si>
   <si>
-    <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
-  </si>
-  <si>
     <t>Initial and parameter field file</t>
   </si>
   <si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>StorageNodeModel</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.crosssections in 0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.rr in 0.2.0</t>
+  </si>
+  <si>
+    <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D3)," ",'Source table'!D3)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E3),ISBLANK('Source table'!F3))," ","["&amp;'Source table'!F3&amp;"]["&amp;'Source table'!E3&amp;"."&amp;'Source table'!F3&amp;"]")</f>
@@ -913,7 +913,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G3)," ","_"&amp;'Source table'!G3&amp;"_")</f>
-        <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
+        <v>_Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127)._</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D22)," ",'Source table'!D22)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E14" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E22),ISBLANK('Source table'!F22))," ","["&amp;'Source table'!F22&amp;"]["&amp;'Source table'!E22&amp;"."&amp;'Source table'!F22&amp;"]")</f>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="F23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
-        <v>_Moved to io.crosssections in 0.1.6._</v>
+        <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="D32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2546,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2555,7 +2555,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -2754,7 +2754,7 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
         <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2870,13 +2870,13 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,12 +2916,12 @@
         <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -2944,15 +2944,15 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
-      </c>
-      <c r="F26" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -2964,15 +2964,15 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -2984,15 +2984,15 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3015,15 +3015,15 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3032,12 +3032,12 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3049,15 +3049,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" t="s">
         <v>80</v>
-      </c>
-      <c r="F32" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3069,15 +3069,15 @@
         <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3089,15 +3089,15 @@
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3109,15 +3109,15 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3129,15 +3129,15 @@
         <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3149,15 +3149,15 @@
         <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3169,15 +3169,15 @@
         <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3189,35 +3189,35 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
-      <c r="F40" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3226,23 +3226,23 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -3251,18 +3251,18 @@
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -3271,18 +3271,18 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3294,20 +3294,20 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -3404,12 +3404,12 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -3418,17 +3418,17 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
@@ -3440,18 +3440,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3463,23 +3463,23 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G60" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -3488,18 +3488,18 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -3508,13 +3508,13 @@
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
         <v>124</v>
-      </c>
-      <c r="F63" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete 0.2.0 changelog + site consistency (#193)
* Complete 0.2.0 changelog + site consistency

* missing topics/tutorials in nav
* Changelog
* mkdocs-macros for easy linking to GitHub and User Manuals.
* list of funtionalities find/replace 0.1.6* -> 0.2.0
* added HYDROLIB logo (but needs a white version)

* autoformat: isort & black

* Added white logo

* #193: more readable + uniform docs headers + intro texts

  Also added support/ref to github issues

* Nice introduction for GitHub README and package website.

 + improved svg logo using paths instead of fonts

* #193: process review comments.

* Fix code smell

Co-authored-by: arthurvd <arthurvd@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2FFE0C-6B07-4B7A-8BB1-43AFDDF35353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DE795-08E2-4835-AD20-F6D8D3171D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>0.1.5</t>
   </si>
   <si>
-    <t>0.1.6*</t>
-  </si>
-  <si>
     <t>UniversalWeir</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Cross section location file</t>
   </si>
   <si>
-    <t>Moved to io.crosssections in 0.1.6.</t>
-  </si>
-  <si>
     <t>hydrolib.core.io.crosssection.models</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
     <t>BuiModel</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.1.6</t>
-  </si>
-  <si>
     <t>Node file 3b_node.tp</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>**RR**</t>
   </si>
   <si>
-    <t>Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127].</t>
-  </si>
-  <si>
     <t>Initial and parameter field file</t>
   </si>
   <si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>StorageNodeModel</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.crosssections in 0.2.0</t>
+  </si>
+  <si>
+    <t>Moved to io.rr in 0.2.0</t>
+  </si>
+  <si>
+    <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D3)," ",'Source table'!D3)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E3),ISBLANK('Source table'!F3))," ","["&amp;'Source table'!F3&amp;"]["&amp;'Source table'!E3&amp;"."&amp;'Source table'!F3&amp;"]")</f>
@@ -913,7 +913,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G3)," ","_"&amp;'Source table'!G3&amp;"_")</f>
-        <v>_Critical bugfix for [#127][https://github.com/Deltares/HYDROLIB-core/issues/127]._</v>
+        <v>_Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127)._</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.1.6_</v>
+        <v>_Moved to io.rr in 0.2.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D7" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D22)," ",'Source table'!D22)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E14" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E22),ISBLANK('Source table'!F22))," ","["&amp;'Source table'!F22&amp;"]["&amp;'Source table'!E22&amp;"."&amp;'Source table'!F22&amp;"]")</f>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="F23" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
-        <v>_Moved to io.crosssections in 0.1.6._</v>
+        <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="D32" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
-        <v>0.1.6*</v>
+        <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2546,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2555,7 +2555,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -2754,7 +2754,7 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
         <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2870,13 +2870,13 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,12 +2916,12 @@
         <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -2944,15 +2944,15 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
         <v>71</v>
-      </c>
-      <c r="F26" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -2964,15 +2964,15 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -2984,15 +2984,15 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3015,15 +3015,15 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3032,12 +3032,12 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3049,15 +3049,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" t="s">
         <v>80</v>
-      </c>
-      <c r="F32" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3069,15 +3069,15 @@
         <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3089,15 +3089,15 @@
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3109,15 +3109,15 @@
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3129,15 +3129,15 @@
         <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3149,15 +3149,15 @@
         <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3169,15 +3169,15 @@
         <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3189,35 +3189,35 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
-      <c r="F40" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3226,23 +3226,23 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F41" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -3251,18 +3251,18 @@
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F43" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -3271,18 +3271,18 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3294,20 +3294,20 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -3404,12 +3404,12 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -3418,17 +3418,17 @@
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
@@ -3440,18 +3440,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3463,23 +3463,23 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G60" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -3488,18 +3488,18 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -3508,13 +3508,13 @@
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="E63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
         <v>124</v>
-      </c>
-      <c r="F63" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small mistake in xlsx (was hiding storage nodes)
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DE795-08E2-4835-AD20-F6D8D3171D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DCA94-3F1A-4A7C-906F-C037CFB44E1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -1253,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,390 +2095,416 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <v>Storage node file</v>
+      </c>
+      <c r="B33" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="C33" t="str">
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <v>0.2.0</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>**Spatial data files**</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C33" t="str">
+      <c r="C34" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E33" s="3" t="str">
+      <c r="E34" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F33" s="3" t="str">
+      <c r="F34" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="str">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>Initial and parameter field file</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C35" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.2.0</v>
       </c>
-      <c r="E34" s="3" t="str">
+      <c r="E35" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
-      <c r="F34" s="3" t="str">
+      <c r="F35" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="str">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>1D field INI files</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C36" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.2.0</v>
       </c>
-      <c r="E35" s="3" t="str">
+      <c r="E36" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
-      <c r="F35" s="3" t="str">
+      <c r="F36" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="str">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>Sample file</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C37" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.1</v>
       </c>
-      <c r="E36" s="3" t="str">
+      <c r="E37" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
-      <c r="F36" s="3" t="str">
+      <c r="F37" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="str">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>**Output**</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C37" t="str">
+      <c r="C38" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E37" s="3" t="str">
+      <c r="E38" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F37" s="3" t="str">
+      <c r="F38" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="str">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>Observation station file (old)</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E38" s="3" t="str">
+      <c r="E39" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F38" s="3" t="str">
+      <c r="F39" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="str">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Observation station file (new)</v>
       </c>
-      <c r="B39" t="str">
+      <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E39" s="3" t="str">
+      <c r="E40" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F39" s="3" t="str">
+      <c r="F40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="str">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>Observation crosssection file (old)</v>
       </c>
-      <c r="B40" t="str">
+      <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E40" s="3" t="str">
+      <c r="E41" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F40" s="3" t="str">
+      <c r="F41" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="str">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Observation crosssection file (new)</v>
       </c>
-      <c r="B41" t="str">
+      <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E41" s="3" t="str">
+      <c r="E42" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F41" s="3" t="str">
+      <c r="F42" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="str">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>History file `_his.nc`</v>
       </c>
-      <c r="B42" t="str">
+      <c r="B43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C42" t="str">
+      <c r="C43" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E42" s="3" t="str">
+      <c r="E43" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F42" s="3" t="str">
+      <c r="F43" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="str">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Map file (old)</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C44" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E43" s="3" t="str">
+      <c r="E44" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F43" s="3" t="str">
+      <c r="F44" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="str">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
-      <c r="B44" t="str">
+      <c r="B45" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C45" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E44" s="3" t="str">
+      <c r="E45" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F44" s="3" t="str">
+      <c r="F45" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="str">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Fourier input file</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B46" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C46" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E45" s="3" t="str">
+      <c r="E46" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F45" s="3" t="str">
+      <c r="F46" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="str">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
-      <c r="B46" t="str">
+      <c r="B47" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C47" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E46" s="3" t="str">
+      <c r="E47" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F46" s="3" t="str">
+      <c r="F47" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="str">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Class map file</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B48" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C48" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E47" s="3" t="str">
+      <c r="E48" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F47" s="3" t="str">
+      <c r="F48" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
@@ -2493,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added obsFile and moved rr subpackages in functionalities list
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DCA94-3F1A-4A7C-906F-C037CFB44E1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
   <si>
     <t>Functionality</t>
   </si>
@@ -385,15 +385,9 @@
     <t>RainfallRunoffModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.fnm.models</t>
-  </si>
-  <si>
     <t>Rainfall .bui file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.bui.models</t>
-  </si>
-  <si>
     <t>BuiModel</t>
   </si>
   <si>
@@ -463,10 +457,28 @@
     <t>Moved to io.crosssections in 0.2.0</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.2.0</t>
-  </si>
-  <si>
     <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obs.models</t>
+  </si>
+  <si>
+    <t>ObservationPointModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.models</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.fnm.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.bui.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.meteo.models</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1146,11 @@
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
+        <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,11 +1172,11 @@
       </c>
       <c r="E4" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
+        <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,7 +1268,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,19 +2294,19 @@
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
@@ -2519,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2584,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2581,7 +2593,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -3058,7 +3070,7 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3232,7 +3244,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
         <v>95</v>
@@ -3243,72 +3255,72 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" t="s">
         <v>126</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>139</v>
-      </c>
-      <c r="E43" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" t="s">
         <v>132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>139</v>
-      </c>
-      <c r="E44" t="s">
-        <v>133</v>
-      </c>
-      <c r="F44" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3320,10 +3332,10 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3347,10 +3359,19 @@
         <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,7 +3470,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3466,18 +3487,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
         <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3489,58 +3510,58 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="F60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" t="s">
         <v>119</v>
       </c>
-      <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>121</v>
-      </c>
-      <c r="F62" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+      <c r="E63" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" t="s">
         <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: Added obsFile and moved rr subpackages in functionalities list for 0.3.0 release
Refs: #274.
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DCA94-3F1A-4A7C-906F-C037CFB44E1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
   <si>
     <t>Functionality</t>
   </si>
@@ -385,15 +385,9 @@
     <t>RainfallRunoffModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.fnm.models</t>
-  </si>
-  <si>
     <t>Rainfall .bui file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.bui.models</t>
-  </si>
-  <si>
     <t>BuiModel</t>
   </si>
   <si>
@@ -463,10 +457,28 @@
     <t>Moved to io.crosssections in 0.2.0</t>
   </si>
   <si>
-    <t>Moved to io.rr in 0.2.0</t>
-  </si>
-  <si>
     <t>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obs.models</t>
+  </si>
+  <si>
+    <t>ObservationPointModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.models</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.fnm.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>Used to be in hydrolib.core.io.bui.models before 0.3.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.rr.meteo.models</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1146,11 @@
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.fnm.models.RainfallRunoffModel]</v>
+        <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,11 +1172,11 @@
       </c>
       <c r="E4" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.bui.models.BuiModel]</v>
+        <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
-        <v>_Moved to io.rr in 0.2.0_</v>
+        <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,7 +1268,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,19 +2294,19 @@
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
@@ -2519,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2584,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
@@ -2581,7 +2593,7 @@
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -3058,7 +3070,7 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3232,7 +3244,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
         <v>95</v>
@@ -3243,72 +3255,72 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" t="s">
         <v>126</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>139</v>
-      </c>
-      <c r="E43" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" t="s">
         <v>132</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>139</v>
-      </c>
-      <c r="E44" t="s">
-        <v>133</v>
-      </c>
-      <c r="F44" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3320,10 +3332,10 @@
         <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3347,10 +3359,19 @@
         <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,7 +3470,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3466,18 +3487,18 @@
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
         <v>114</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -3489,58 +3510,58 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="F60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" t="s">
         <v>119</v>
       </c>
-      <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>121</v>
-      </c>
-      <c r="F62" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+      <c r="E63" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" t="s">
         <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update list of supported functionalities for 0.3.1 release
Added:
* t3d
* vector bc
* observation cross section
* all already-supported bc function types in earlier releases
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17C55D-05C7-4B4E-ADB6-65EACAF64AA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Functionality</t>
   </si>
@@ -479,6 +479,57 @@
   </si>
   <si>
     <t>hydrolib.core.io.rr.meteo.models</t>
+  </si>
+  <si>
+    <t>** timeSeries</t>
+  </si>
+  <si>
+    <t>** harmonic (-Correction)</t>
+  </si>
+  <si>
+    <t>** astronomic (-Correction)</t>
+  </si>
+  <si>
+    <t>** t3D</t>
+  </si>
+  <si>
+    <t>** QHTable</t>
+  </si>
+  <si>
+    <t>** constant</t>
+  </si>
+  <si>
+    <t>** vector quantities</t>
+  </si>
+  <si>
+    <t>TimeSeries</t>
+  </si>
+  <si>
+    <t>T3D</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>0.3.1</t>
+  </si>
+  <si>
+    <t>VectorQuantityUnitPairs</t>
+  </si>
+  <si>
+    <t>QHTable</t>
+  </si>
+  <si>
+    <t>Astronomic</t>
+  </si>
+  <si>
+    <t>Harmonic</t>
+  </si>
+  <si>
+    <t>ObservationCrossSectionModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obscrosssection.models</t>
   </si>
 </sst>
 </file>
@@ -844,7 +895,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,157 +1154,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A65)," ",'Source table'!A65)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D65)," ",'Source table'!D65)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E65),ISBLANK('Source table'!F65))," ","["&amp;'Source table'!F65&amp;"]["&amp;'Source table'!E65&amp;"."&amp;'Source table'!F65&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G65)," ","_"&amp;'Source table'!G65&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
+        <f>IF(ISBLANK('Source table'!A66)," ",'Source table'!A66)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
+        <f>IF(ISBLANK('Source table'!D66)," ",'Source table'!D66)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E66),ISBLANK('Source table'!F66))," ","["&amp;'Source table'!F66&amp;"]["&amp;'Source table'!E66&amp;"."&amp;'Source table'!F66&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G66)," ","_"&amp;'Source table'!G66&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
+        <f>IF(ISBLANK('Source table'!A67)," ",'Source table'!A67)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
+        <f>IF(ISBLANK('Source table'!D67)," ",'Source table'!D67)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
+        <f>IF(ISBLANK('Source table'!A68)," ",'Source table'!A68)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
+        <f>IF(ISBLANK('Source table'!D68)," ",'Source table'!D68)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E68),ISBLANK('Source table'!F68))," ","["&amp;'Source table'!F68&amp;"]["&amp;'Source table'!E68&amp;"."&amp;'Source table'!F68&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G68)," ","_"&amp;'Source table'!G68&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
+        <f>IF(ISBLANK('Source table'!A69)," ",'Source table'!A69)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
+        <f>IF(ISBLANK('Source table'!D69)," ",'Source table'!D69)</f>
         <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <f>IF(ISBLANK('Source table'!A70)," ",'Source table'!A70)</f>
         <v>Link file 3b_link.tp</v>
       </c>
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <f>IF(ISBLANK('Source table'!D70)," ",'Source table'!D70)</f>
         <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
         <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1267,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,677 +1898,677 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
+        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>**Cross section files**</v>
       </c>
       <c r="B23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D31)," ",'Source table'!D31)</f>
+        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E31),ISBLANK('Source table'!F31))," ","["&amp;'Source table'!F31&amp;"]["&amp;'Source table'!E31&amp;"."&amp;'Source table'!F31&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
         <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
+        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section definition file</v>
       </c>
       <c r="B24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D32)," ",'Source table'!D32)</f>
+        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
         <v>0.1.1</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E32),ISBLANK('Source table'!F32))," ","["&amp;'Source table'!F32&amp;"]["&amp;'Source table'!E32&amp;"."&amp;'Source table'!F32&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
         <v>[CrossDefModel][hydrolib.core.io.crosssection.models.CrossDefModel]</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G32)," ","_"&amp;'Source table'!G32&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
+        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>* Circle</v>
       </c>
       <c r="B25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D33)," ",'Source table'!D33)</f>
+        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
         <v>0.1.5</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E33),ISBLANK('Source table'!F33))," ","["&amp;'Source table'!F33&amp;"]["&amp;'Source table'!E33&amp;"."&amp;'Source table'!F33&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
         <v>[CircleCrsDef][hydrolib.core.io.crosssection.models.CircleCrsDef]</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G33)," ","_"&amp;'Source table'!G33&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
         <v>* Rectangle</v>
       </c>
       <c r="B26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D34)," ",'Source table'!D34)</f>
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
         <v>0.1.5</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E34),ISBLANK('Source table'!F34))," ","["&amp;'Source table'!F34&amp;"]["&amp;'Source table'!E34&amp;"."&amp;'Source table'!F34&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
         <v>[RectangleCrsDef][hydrolib.core.io.crosssection.models.RectangleCrsDef]</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G34)," ","_"&amp;'Source table'!G34&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>* Tabulated river</v>
       </c>
       <c r="B27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D35)," ",'Source table'!D35)</f>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v>0.1.5</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E35),ISBLANK('Source table'!F35))," ","["&amp;'Source table'!F35&amp;"]["&amp;'Source table'!E35&amp;"."&amp;'Source table'!F35&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v>[ZWRiverCrsDef][hydrolib.core.io.crosssection.models.ZWRiverCrsDef]</v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G35)," ","_"&amp;'Source table'!G35&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>* ZW (tabulated)</v>
       </c>
       <c r="B28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D36)," ",'Source table'!D36)</f>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.1.5</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E36),ISBLANK('Source table'!F36))," ","["&amp;'Source table'!F36&amp;"]["&amp;'Source table'!E36&amp;"."&amp;'Source table'!F36&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[ZWCrsDef][hydrolib.core.io.crosssection.models.ZWCrsDef]</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G36)," ","_"&amp;'Source table'!G36&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>* XYZ</v>
       </c>
       <c r="B29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D37)," ",'Source table'!D37)</f>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.1.5</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E37),ISBLANK('Source table'!F37))," ","["&amp;'Source table'!F37&amp;"]["&amp;'Source table'!E37&amp;"."&amp;'Source table'!F37&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[XYZCrsDef][hydrolib.core.io.crosssection.models.XYZCrsDef]</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G37)," ","_"&amp;'Source table'!G37&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>* YZ</v>
       </c>
       <c r="B30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.5</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[YZCrsDef][hydrolib.core.io.crosssection.models.YZCrsDef]</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>Cross section location file</v>
       </c>
       <c r="B31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v>0.1.1</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v>[CrossLocModel][hydrolib.core.io.crosssection.models.CrossLocModel]</v>
       </c>
       <c r="F31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>1D roughness file</v>
       </c>
       <c r="B32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v>[FrictionModel][hydrolib.core.io.friction.models.FrictionModel]</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v>0.2.0</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>**Spatial data files**</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Initial and parameter field file</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>1D field INI files</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v>0.2.0</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Sample file</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v>0.1.1</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>**Output**</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Observation station file (old)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Observation station file (new)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Observation crosssection file (old)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>Observation crosssection file (new)</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <v>0.3.1</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <v>[ObservationCrossSectionModel][hydrolib.core.io.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>History file `_his.nc`</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Map file (old)</v>
       </c>
       <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>Fourier input file</v>
       </c>
       <c r="B46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E47" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
         <v>Class map file</v>
       </c>
       <c r="B48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E48" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
@@ -2529,10 +2580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,7 +2866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2826,7 +2877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2846,7 +2897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2886,7 +2937,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2897,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2917,7 +2968,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2937,7 +2988,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2968,7 +3019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2988,7 +3039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3008,7 +3059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -3028,7 +3079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3039,7 +3090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -3059,9 +3110,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3069,13 +3120,19 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3087,15 +3144,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3104,18 +3161,18 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3124,18 +3181,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3144,18 +3201,18 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3164,18 +3221,18 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3184,18 +3241,18 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3203,19 +3260,13 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3230,208 +3281,262 @@
         <v>78</v>
       </c>
       <c r="F39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
         <v>137</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E47" t="s">
         <v>95</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>134</v>
       </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>137</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E48" t="s">
         <v>135</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F48" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3442,132 +3547,227 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
-        <v>110</v>
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>110</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E59" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" t="s">
-        <v>144</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
-        <v>57</v>
-      </c>
-      <c r="E60" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" t="s">
-        <v>116</v>
-      </c>
-      <c r="G60" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>137</v>
-      </c>
-      <c r="E62" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" t="s">
-        <v>121</v>
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" t="s">
+        <v>114</v>
+      </c>
+      <c r="G66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>120</v>
       </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>137</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>119</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F70" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G59" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G70" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
docs: Update list of supported functionalities for 0.3.1 release (#387)
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D187E0-D86F-4FDE-A702-B70706D2A865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17C55D-05C7-4B4E-ADB6-65EACAF64AA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Functionality</t>
   </si>
@@ -479,6 +479,57 @@
   </si>
   <si>
     <t>hydrolib.core.io.rr.meteo.models</t>
+  </si>
+  <si>
+    <t>** timeSeries</t>
+  </si>
+  <si>
+    <t>** harmonic (-Correction)</t>
+  </si>
+  <si>
+    <t>** astronomic (-Correction)</t>
+  </si>
+  <si>
+    <t>** t3D</t>
+  </si>
+  <si>
+    <t>** QHTable</t>
+  </si>
+  <si>
+    <t>** constant</t>
+  </si>
+  <si>
+    <t>** vector quantities</t>
+  </si>
+  <si>
+    <t>TimeSeries</t>
+  </si>
+  <si>
+    <t>T3D</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>0.3.1</t>
+  </si>
+  <si>
+    <t>VectorQuantityUnitPairs</t>
+  </si>
+  <si>
+    <t>QHTable</t>
+  </si>
+  <si>
+    <t>Astronomic</t>
+  </si>
+  <si>
+    <t>Harmonic</t>
+  </si>
+  <si>
+    <t>ObservationCrossSectionModel</t>
+  </si>
+  <si>
+    <t>hydrolib.core.io.obscrosssection.models</t>
   </si>
 </sst>
 </file>
@@ -844,7 +895,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,157 +1154,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A65)," ",'Source table'!A65)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D65)," ",'Source table'!D65)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E65),ISBLANK('Source table'!F65))," ","["&amp;'Source table'!F65&amp;"]["&amp;'Source table'!E65&amp;"."&amp;'Source table'!F65&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G65)," ","_"&amp;'Source table'!G65&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
+        <f>IF(ISBLANK('Source table'!A66)," ",'Source table'!A66)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
+        <f>IF(ISBLANK('Source table'!D66)," ",'Source table'!D66)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E66),ISBLANK('Source table'!F66))," ","["&amp;'Source table'!F66&amp;"]["&amp;'Source table'!E66&amp;"."&amp;'Source table'!F66&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G66)," ","_"&amp;'Source table'!G66&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
+        <f>IF(ISBLANK('Source table'!A67)," ",'Source table'!A67)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
+        <f>IF(ISBLANK('Source table'!D67)," ",'Source table'!D67)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
+        <f>IF(ISBLANK('Source table'!A68)," ",'Source table'!A68)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
+        <f>IF(ISBLANK('Source table'!D68)," ",'Source table'!D68)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E68),ISBLANK('Source table'!F68))," ","["&amp;'Source table'!F68&amp;"]["&amp;'Source table'!E68&amp;"."&amp;'Source table'!F68&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G68)," ","_"&amp;'Source table'!G68&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
+        <f>IF(ISBLANK('Source table'!A69)," ",'Source table'!A69)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
+        <f>IF(ISBLANK('Source table'!D69)," ",'Source table'!D69)</f>
         <v>0.2.0</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <f>IF(ISBLANK('Source table'!A70)," ",'Source table'!A70)</f>
         <v>Link file 3b_link.tp</v>
       </c>
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <f>IF(ISBLANK('Source table'!D70)," ",'Source table'!D70)</f>
         <v>0.2.0</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
         <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1267,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,677 +1898,677 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
+        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
         <v>**Cross section files**</v>
       </c>
       <c r="B23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D31)," ",'Source table'!D31)</f>
+        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E31),ISBLANK('Source table'!F31))," ","["&amp;'Source table'!F31&amp;"]["&amp;'Source table'!E31&amp;"."&amp;'Source table'!F31&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F23" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
         <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A32)," ",'Source table'!A32)</f>
+        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
         <v>Cross section definition file</v>
       </c>
       <c r="B24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C32,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D32)," ",'Source table'!D32)</f>
+        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
         <v>0.1.1</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E32),ISBLANK('Source table'!F32))," ","["&amp;'Source table'!F32&amp;"]["&amp;'Source table'!E32&amp;"."&amp;'Source table'!F32&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
         <v>[CrossDefModel][hydrolib.core.io.crosssection.models.CrossDefModel]</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G32)," ","_"&amp;'Source table'!G32&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A33)," ",'Source table'!A33)</f>
+        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>* Circle</v>
       </c>
       <c r="B25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C33,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D33)," ",'Source table'!D33)</f>
+        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
         <v>0.1.5</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E33),ISBLANK('Source table'!F33))," ","["&amp;'Source table'!F33&amp;"]["&amp;'Source table'!E33&amp;"."&amp;'Source table'!F33&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
         <v>[CircleCrsDef][hydrolib.core.io.crosssection.models.CircleCrsDef]</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G33)," ","_"&amp;'Source table'!G33&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A34)," ",'Source table'!A34)</f>
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
         <v>* Rectangle</v>
       </c>
       <c r="B26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C34,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D34)," ",'Source table'!D34)</f>
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
         <v>0.1.5</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E34),ISBLANK('Source table'!F34))," ","["&amp;'Source table'!F34&amp;"]["&amp;'Source table'!E34&amp;"."&amp;'Source table'!F34&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
         <v>[RectangleCrsDef][hydrolib.core.io.crosssection.models.RectangleCrsDef]</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G34)," ","_"&amp;'Source table'!G34&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A35)," ",'Source table'!A35)</f>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>* Tabulated river</v>
       </c>
       <c r="B27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C35,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D35)," ",'Source table'!D35)</f>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v>0.1.5</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E35),ISBLANK('Source table'!F35))," ","["&amp;'Source table'!F35&amp;"]["&amp;'Source table'!E35&amp;"."&amp;'Source table'!F35&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v>[ZWRiverCrsDef][hydrolib.core.io.crosssection.models.ZWRiverCrsDef]</v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G35)," ","_"&amp;'Source table'!G35&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A36)," ",'Source table'!A36)</f>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>* ZW (tabulated)</v>
       </c>
       <c r="B28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C36,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D36)," ",'Source table'!D36)</f>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.1.5</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E36),ISBLANK('Source table'!F36))," ","["&amp;'Source table'!F36&amp;"]["&amp;'Source table'!E36&amp;"."&amp;'Source table'!F36&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[ZWCrsDef][hydrolib.core.io.crosssection.models.ZWCrsDef]</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G36)," ","_"&amp;'Source table'!G36&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A37)," ",'Source table'!A37)</f>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>* XYZ</v>
       </c>
       <c r="B29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C37,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D37)," ",'Source table'!D37)</f>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.1.5</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E37),ISBLANK('Source table'!F37))," ","["&amp;'Source table'!F37&amp;"]["&amp;'Source table'!E37&amp;"."&amp;'Source table'!F37&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[XYZCrsDef][hydrolib.core.io.crosssection.models.XYZCrsDef]</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G37)," ","_"&amp;'Source table'!G37&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>* YZ</v>
       </c>
       <c r="B30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.5</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[YZCrsDef][hydrolib.core.io.crosssection.models.YZCrsDef]</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>Cross section location file</v>
       </c>
       <c r="B31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v>0.1.1</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v>[CrossLocModel][hydrolib.core.io.crosssection.models.CrossLocModel]</v>
       </c>
       <c r="F31" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>1D roughness file</v>
       </c>
       <c r="B32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v>0.2.0</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v>[FrictionModel][hydrolib.core.io.friction.models.FrictionModel]</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v>0.2.0</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>**Spatial data files**</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Initial and parameter field file</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v>0.2.0</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>1D field INI files</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v>0.2.0</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Sample file</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v>0.1.1</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>**Output**</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Observation station file (old)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>Observation station file (new)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v>0.3.0</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Observation crosssection file (old)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>Observation crosssection file (new)</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:material-close-box:</v>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <v>0.3.1</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <v>[ObservationCrossSectionModel][hydrolib.core.io.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>History file `_his.nc`</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Map file (old)</v>
       </c>
       <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F44" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F45" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>Fourier input file</v>
       </c>
       <c r="B46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F46" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E47" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F47" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
         <v>Class map file</v>
       </c>
       <c r="B48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E48" s="3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
@@ -2529,10 +2580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,7 +2866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2826,7 +2877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2846,7 +2897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2886,7 +2937,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2897,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2917,7 +2968,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2937,7 +2988,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2968,7 +3019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2988,7 +3039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -3008,7 +3059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -3028,7 +3079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3039,7 +3090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -3059,9 +3110,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3069,13 +3120,19 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="G31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3087,15 +3144,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3104,18 +3161,18 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3124,18 +3181,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3144,18 +3201,18 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3164,18 +3221,18 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3184,18 +3241,18 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3203,19 +3260,13 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3230,208 +3281,262 @@
         <v>78</v>
       </c>
       <c r="F39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
         <v>137</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E47" t="s">
         <v>95</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>134</v>
       </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>137</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E48" t="s">
         <v>135</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F48" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3442,132 +3547,227 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
-        <v>110</v>
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>110</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E59" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" t="s">
-        <v>144</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
-        <v>57</v>
-      </c>
-      <c r="E60" t="s">
-        <v>146</v>
-      </c>
-      <c r="F60" t="s">
-        <v>116</v>
-      </c>
-      <c r="G60" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>137</v>
-      </c>
-      <c r="E62" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" t="s">
-        <v>121</v>
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" t="s">
+        <v>114</v>
+      </c>
+      <c r="G66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>120</v>
       </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>137</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>119</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F70" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G59" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G70" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the dflowfm and rr namespaces
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HydroLib\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52135687-B8E6-4A63-80AA-FFCEA5299A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE463E1-2152-4571-8934-12818225F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -162,18 +162,9 @@
     <t>Weir</t>
   </si>
   <si>
-    <t>hydrolib.core.io.mdu.models</t>
-  </si>
-  <si>
-    <t>hydrolib.core.io.structure.models</t>
-  </si>
-  <si>
     <t>FMModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.net.models</t>
-  </si>
-  <si>
     <t>Mesh2d</t>
   </si>
   <si>
@@ -252,9 +243,6 @@
     <t>* Meteo</t>
   </si>
   <si>
-    <t>hydrolib.core.io.ext.models</t>
-  </si>
-  <si>
     <t>ExtModel</t>
   </si>
   <si>
@@ -270,15 +258,9 @@
     <t>ForcingModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.bc.models</t>
-  </si>
-  <si>
     <t>Cross section location file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.crosssection.models</t>
-  </si>
-  <si>
     <t>CrossLocModel</t>
   </si>
   <si>
@@ -327,9 +309,6 @@
     <t>1D roughness file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.friction.models</t>
-  </si>
-  <si>
     <t>FrictionModel</t>
   </si>
   <si>
@@ -399,9 +378,6 @@
     <t>**Topology layer**</t>
   </si>
   <si>
-    <t>hydrolib.core.io.rr.topology.models</t>
-  </si>
-  <si>
     <t>Link file 3b_link.tp</t>
   </si>
   <si>
@@ -417,27 +393,18 @@
     <t>Initial and parameter field file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.inifield.models</t>
-  </si>
-  <si>
     <t>IniFieldModel</t>
   </si>
   <si>
     <t>Sample file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.xyz.models</t>
-  </si>
-  <si>
     <t>XYZModel</t>
   </si>
   <si>
     <t>1D field INI files</t>
   </si>
   <si>
-    <t>hydrolib.core.io.onedfield.models</t>
-  </si>
-  <si>
     <t>OneDFieldModel</t>
   </si>
   <si>
@@ -447,9 +414,6 @@
     <t>Storage node file</t>
   </si>
   <si>
-    <t>hydrolib.core.io.storagenode.models</t>
-  </si>
-  <si>
     <t>StorageNodeModel</t>
   </si>
   <si>
@@ -465,24 +429,15 @@
     <t>0.3.0</t>
   </si>
   <si>
-    <t>hydrolib.core.io.obs.models</t>
-  </si>
-  <si>
     <t>ObservationPointModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.rr.models</t>
-  </si>
-  <si>
     <t>Used to be in hydrolib.core.io.fnm.models before 0.3.0</t>
   </si>
   <si>
     <t>Used to be in hydrolib.core.io.bui.models before 0.3.0</t>
   </si>
   <si>
-    <t>hydrolib.core.io.rr.meteo.models</t>
-  </si>
-  <si>
     <t>** timeSeries</t>
   </si>
   <si>
@@ -531,10 +486,55 @@
     <t>ObservationCrossSectionModel</t>
   </si>
   <si>
-    <t>hydrolib.core.io.obscrosssection.models</t>
-  </si>
-  <si>
     <t>hydrolib.core.dimr.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.mdu.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.net.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.structure.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.ext.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.bc.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.crosssection.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.friction.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.storagenode.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.inifield.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.onedfield.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.xyz.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.obs.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.obscrosssection.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.rr.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.rr.meteo.models</t>
+  </si>
+  <si>
+    <t>hydrolib.core.rr.topology.models</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E66),ISBLANK('Source table'!F66))," ","["&amp;'Source table'!F66&amp;"]["&amp;'Source table'!E66&amp;"."&amp;'Source table'!F66&amp;"]")</f>
-        <v>[RainfallRunoffModel][hydrolib.core.io.rr.models.RainfallRunoffModel]</v>
+        <v>[RainfallRunoffModel][hydrolib.core.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" t="str">
         <f>IF(ISBLANK('Source table'!G66)," ","_"&amp;'Source table'!G66&amp;"_")</f>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="E4" t="str">
         <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
-        <v>[BuiModel][hydrolib.core.io.rr.meteo.models.BuiModel]</v>
+        <v>[BuiModel][hydrolib.core.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" t="str">
         <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E6" t="str">
         <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
-        <v>[NodeFile][hydrolib.core.io.rr.topology.models.NodeFile]</v>
+        <v>[NodeFile][hydrolib.core.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="E7" t="str">
         <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
-        <v>[LinkFile][hydrolib.core.io.rr.topology.models.LinkFile]</v>
+        <v>[LinkFile][hydrolib.core.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="E3" t="str">
         <f>IF(OR(ISBLANK('Source table'!E11),ISBLANK('Source table'!F11))," ","["&amp;'Source table'!F11&amp;"]["&amp;'Source table'!E11&amp;"."&amp;'Source table'!F11&amp;"]")</f>
-        <v>[FMModel][hydrolib.core.io.mdu.models.FMModel]</v>
+        <v>[FMModel][hydrolib.core.dflowfm.mdu.models.FMModel]</v>
       </c>
       <c r="F3" t="str">
         <f>IF(ISBLANK('Source table'!G11)," ","_"&amp;'Source table'!G11&amp;"_")</f>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="E4" t="str">
         <f>IF(OR(ISBLANK('Source table'!E12),ISBLANK('Source table'!F12))," ","["&amp;'Source table'!F12&amp;"]["&amp;'Source table'!E12&amp;"."&amp;'Source table'!F12&amp;"]")</f>
-        <v>[Mesh2d][hydrolib.core.io.net.models.Mesh2d]</v>
+        <v>[Mesh2d][hydrolib.core.dflowfm.net.models.Mesh2d]</v>
       </c>
       <c r="F4" t="str">
         <f>IF(ISBLANK('Source table'!G12)," ","_"&amp;'Source table'!G12&amp;"_")</f>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="E5" t="str">
         <f>IF(OR(ISBLANK('Source table'!E13),ISBLANK('Source table'!F13))," ","["&amp;'Source table'!F13&amp;"]["&amp;'Source table'!E13&amp;"."&amp;'Source table'!F13&amp;"]")</f>
-        <v>[StructureModel][hydrolib.core.io.structure.models.StructureModel]</v>
+        <v>[StructureModel][hydrolib.core.dflowfm.structure.models.StructureModel]</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISBLANK('Source table'!G13)," ","_"&amp;'Source table'!G13&amp;"_")</f>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E6" t="str">
         <f>IF(OR(ISBLANK('Source table'!E14),ISBLANK('Source table'!F14))," ","["&amp;'Source table'!F14&amp;"]["&amp;'Source table'!E14&amp;"."&amp;'Source table'!F14&amp;"]")</f>
-        <v>[Weir][hydrolib.core.io.structure.models.Weir]</v>
+        <v>[Weir][hydrolib.core.dflowfm.structure.models.Weir]</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISBLANK('Source table'!G14)," ","_"&amp;'Source table'!G14&amp;"_")</f>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="E7" t="str">
         <f>IF(OR(ISBLANK('Source table'!E15),ISBLANK('Source table'!F15))," ","["&amp;'Source table'!F15&amp;"]["&amp;'Source table'!E15&amp;"."&amp;'Source table'!F15&amp;"]")</f>
-        <v>[UniversalWeir][hydrolib.core.io.structure.models.UniversalWeir]</v>
+        <v>[UniversalWeir][hydrolib.core.dflowfm.structure.models.UniversalWeir]</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISBLANK('Source table'!G15)," ","_"&amp;'Source table'!G15&amp;"_")</f>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="E8" t="str">
         <f>IF(OR(ISBLANK('Source table'!E16),ISBLANK('Source table'!F16))," ","["&amp;'Source table'!F16&amp;"]["&amp;'Source table'!E16&amp;"."&amp;'Source table'!F16&amp;"]")</f>
-        <v>[Culvert][hydrolib.core.io.structure.models.Culvert]</v>
+        <v>[Culvert][hydrolib.core.dflowfm.structure.models.Culvert]</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISBLANK('Source table'!G16)," ","_"&amp;'Source table'!G16&amp;"_")</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="E10" t="str">
         <f>IF(OR(ISBLANK('Source table'!E18),ISBLANK('Source table'!F18))," ","["&amp;'Source table'!F18&amp;"]["&amp;'Source table'!E18&amp;"."&amp;'Source table'!F18&amp;"]")</f>
-        <v>[Bridge][hydrolib.core.io.structure.models.Bridge]</v>
+        <v>[Bridge][hydrolib.core.dflowfm.structure.models.Bridge]</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISBLANK('Source table'!G18)," ","_"&amp;'Source table'!G18&amp;"_")</f>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="E11" t="str">
         <f>IF(OR(ISBLANK('Source table'!E19),ISBLANK('Source table'!F19))," ","["&amp;'Source table'!F19&amp;"]["&amp;'Source table'!E19&amp;"."&amp;'Source table'!F19&amp;"]")</f>
-        <v>[Pump][hydrolib.core.io.structure.models.Pump]</v>
+        <v>[Pump][hydrolib.core.dflowfm.structure.models.Pump]</v>
       </c>
       <c r="F11" t="str">
         <f>IF(ISBLANK('Source table'!G19)," ","_"&amp;'Source table'!G19&amp;"_")</f>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="E12" t="str">
         <f>IF(OR(ISBLANK('Source table'!E20),ISBLANK('Source table'!F20))," ","["&amp;'Source table'!F20&amp;"]["&amp;'Source table'!E20&amp;"."&amp;'Source table'!F20&amp;"]")</f>
-        <v>[Orifice][hydrolib.core.io.structure.models.Orifice]</v>
+        <v>[Orifice][hydrolib.core.dflowfm.structure.models.Orifice]</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISBLANK('Source table'!G20)," ","_"&amp;'Source table'!G20&amp;"_")</f>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="E14" t="str">
         <f>IF(OR(ISBLANK('Source table'!E22),ISBLANK('Source table'!F22))," ","["&amp;'Source table'!F22&amp;"]["&amp;'Source table'!E22&amp;"."&amp;'Source table'!F22&amp;"]")</f>
-        <v>[GeneralStructure][hydrolib.core.io.structure.models.GeneralStructure]</v>
+        <v>[GeneralStructure][hydrolib.core.dflowfm.structure.models.GeneralStructure]</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISBLANK('Source table'!G22)," ","_"&amp;'Source table'!G22&amp;"_")</f>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="E15" t="str">
         <f>IF(OR(ISBLANK('Source table'!E23),ISBLANK('Source table'!F23))," ","["&amp;'Source table'!F23&amp;"]["&amp;'Source table'!E23&amp;"."&amp;'Source table'!F23&amp;"]")</f>
-        <v>[Dambreak][hydrolib.core.io.structure.models.Dambreak]</v>
+        <v>[Dambreak][hydrolib.core.dflowfm.structure.models.Dambreak]</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISBLANK('Source table'!G23)," ","_"&amp;'Source table'!G23&amp;"_")</f>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="E16" t="str">
         <f>IF(OR(ISBLANK('Source table'!E24),ISBLANK('Source table'!F24))," ","["&amp;'Source table'!F24&amp;"]["&amp;'Source table'!E24&amp;"."&amp;'Source table'!F24&amp;"]")</f>
-        <v>[Compound][hydrolib.core.io.structure.models.Compound]</v>
+        <v>[Compound][hydrolib.core.dflowfm.structure.models.Compound]</v>
       </c>
       <c r="F16" t="str">
         <f>IF(ISBLANK('Source table'!G24)," ","_"&amp;'Source table'!G24&amp;"_")</f>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="E18" t="str">
         <f>IF(OR(ISBLANK('Source table'!E26),ISBLANK('Source table'!F26))," ","["&amp;'Source table'!F26&amp;"]["&amp;'Source table'!E26&amp;"."&amp;'Source table'!F26&amp;"]")</f>
-        <v>[ExtModel][hydrolib.core.io.ext.models.ExtModel]</v>
+        <v>[ExtModel][hydrolib.core.dflowfm.ext.models.ExtModel]</v>
       </c>
       <c r="F18" t="str">
         <f>IF(ISBLANK('Source table'!G26)," ","_"&amp;'Source table'!G26&amp;"_")</f>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="E19" t="str">
         <f>IF(OR(ISBLANK('Source table'!E27),ISBLANK('Source table'!F27))," ","["&amp;'Source table'!F27&amp;"]["&amp;'Source table'!E27&amp;"."&amp;'Source table'!F27&amp;"]")</f>
-        <v>[Boundary][hydrolib.core.io.ext.models.Boundary]</v>
+        <v>[Boundary][hydrolib.core.dflowfm.ext.models.Boundary]</v>
       </c>
       <c r="F19" t="str">
         <f>IF(ISBLANK('Source table'!G27)," ","_"&amp;'Source table'!G27&amp;"_")</f>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="E20" t="str">
         <f>IF(OR(ISBLANK('Source table'!E28),ISBLANK('Source table'!F28))," ","["&amp;'Source table'!F28&amp;"]["&amp;'Source table'!E28&amp;"."&amp;'Source table'!F28&amp;"]")</f>
-        <v>[Lateral][hydrolib.core.io.ext.models.Lateral]</v>
+        <v>[Lateral][hydrolib.core.dflowfm.ext.models.Lateral]</v>
       </c>
       <c r="F20" t="str">
         <f>IF(ISBLANK('Source table'!G28)," ","_"&amp;'Source table'!G28&amp;"_")</f>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="E22" t="str">
         <f>IF(OR(ISBLANK('Source table'!E30),ISBLANK('Source table'!F30))," ","["&amp;'Source table'!F30&amp;"]["&amp;'Source table'!E30&amp;"."&amp;'Source table'!F30&amp;"]")</f>
-        <v>[ForcingModel][hydrolib.core.io.bc.models.ForcingModel]</v>
+        <v>[ForcingModel][hydrolib.core.dflowfm.bc.models.ForcingModel]</v>
       </c>
       <c r="F22" t="str">
         <f>IF(ISBLANK('Source table'!G30)," ","_"&amp;'Source table'!G30&amp;"_")</f>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="E24" t="str">
         <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
-        <v>[CrossDefModel][hydrolib.core.io.crosssection.models.CrossDefModel]</v>
+        <v>[CrossDefModel][hydrolib.core.dflowfm.crosssection.models.CrossDefModel]</v>
       </c>
       <c r="F24" t="str">
         <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="E25" t="str">
         <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
-        <v>[CircleCrsDef][hydrolib.core.io.crosssection.models.CircleCrsDef]</v>
+        <v>[CircleCrsDef][hydrolib.core.dflowfm.crosssection.models.CircleCrsDef]</v>
       </c>
       <c r="F25" t="str">
         <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="E26" t="str">
         <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
-        <v>[RectangleCrsDef][hydrolib.core.io.crosssection.models.RectangleCrsDef]</v>
+        <v>[RectangleCrsDef][hydrolib.core.dflowfm.crosssection.models.RectangleCrsDef]</v>
       </c>
       <c r="F26" t="str">
         <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="E27" t="str">
         <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
-        <v>[ZWRiverCrsDef][hydrolib.core.io.crosssection.models.ZWRiverCrsDef]</v>
+        <v>[ZWRiverCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWRiverCrsDef]</v>
       </c>
       <c r="F27" t="str">
         <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="E28" t="str">
         <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
-        <v>[ZWCrsDef][hydrolib.core.io.crosssection.models.ZWCrsDef]</v>
+        <v>[ZWCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWCrsDef]</v>
       </c>
       <c r="F28" t="str">
         <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="E29" t="str">
         <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
-        <v>[XYZCrsDef][hydrolib.core.io.crosssection.models.XYZCrsDef]</v>
+        <v>[XYZCrsDef][hydrolib.core.dflowfm.crosssection.models.XYZCrsDef]</v>
       </c>
       <c r="F29" t="str">
         <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E30" t="str">
         <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
-        <v>[YZCrsDef][hydrolib.core.io.crosssection.models.YZCrsDef]</v>
+        <v>[YZCrsDef][hydrolib.core.dflowfm.crosssection.models.YZCrsDef]</v>
       </c>
       <c r="F30" t="str">
         <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="E31" t="str">
         <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
-        <v>[CrossLocModel][hydrolib.core.io.crosssection.models.CrossLocModel]</v>
+        <v>[CrossLocModel][hydrolib.core.dflowfm.crosssection.models.CrossLocModel]</v>
       </c>
       <c r="F31" t="str">
         <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
@@ -2153,7 +2153,7 @@
       </c>
       <c r="E32" t="str">
         <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
-        <v>[FrictionModel][hydrolib.core.io.friction.models.FrictionModel]</v>
+        <v>[FrictionModel][hydrolib.core.dflowfm.friction.models.FrictionModel]</v>
       </c>
       <c r="F32" t="str">
         <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="E33" t="str">
         <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
-        <v>[StorageNodeModel][hydrolib.core.io.storagenode.models.StorageNodeModel]</v>
+        <v>[StorageNodeModel][hydrolib.core.dflowfm.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" t="str">
         <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="E35" t="str">
         <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
-        <v>[IniFieldModel][hydrolib.core.io.inifield.models.IniFieldModel]</v>
+        <v>[IniFieldModel][hydrolib.core.dflowfm.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F35" t="str">
         <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="E36" t="str">
         <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
-        <v>[OneDFieldModel][hydrolib.core.io.onedfield.models.OneDFieldModel]</v>
+        <v>[OneDFieldModel][hydrolib.core.dflowfm.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F36" t="str">
         <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="E37" t="str">
         <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
-        <v>[XYZModel][hydrolib.core.io.xyz.models.XYZModel]</v>
+        <v>[XYZModel][hydrolib.core.dflowfm.xyz.models.XYZModel]</v>
       </c>
       <c r="F37" t="str">
         <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="E40" t="str">
         <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
-        <v>[ObservationPointModel][hydrolib.core.io.obs.models.ObservationPointModel]</v>
+        <v>[ObservationPointModel][hydrolib.core.dflowfm.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" t="str">
         <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="E42" t="str">
         <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
-        <v>[ObservationCrossSectionModel][hydrolib.core.io.obscrosssection.models.ObservationCrossSectionModel]</v>
+        <v>[ObservationCrossSectionModel][hydrolib.core.dflowfm.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
       <c r="F42" t="str">
         <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
@@ -2586,8 +2586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E3:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,16 +2639,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -2685,7 +2685,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
@@ -2702,7 +2702,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,10 +2719,10 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2739,7 +2739,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -2764,10 +2764,10 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" t="s">
         <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2784,15 +2784,15 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -2804,15 +2804,15 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -2824,7 +2824,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F14" t="s">
         <v>38</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -2844,15 +2844,15 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -2864,15 +2864,15 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -2892,18 +2892,18 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -2915,15 +2915,15 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -2935,15 +2935,15 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -2963,38 +2963,38 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
-      </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3006,15 +3006,15 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3037,15 +3037,15 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3057,15 +3057,15 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3077,15 +3077,15 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3108,15 +3108,15 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3128,15 +3128,15 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3148,15 +3148,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F32" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3168,15 +3168,15 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3185,18 +3185,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F34" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3208,15 +3208,15 @@
         <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F35" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3228,35 +3228,35 @@
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="F36" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" t="s">
         <v>152</v>
       </c>
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>156</v>
-      </c>
-      <c r="E37" t="s">
-        <v>75</v>
-      </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3265,12 +3265,12 @@
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3282,55 +3282,55 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>153</v>
+      </c>
+      <c r="F40" t="s">
         <v>81</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -3339,18 +3339,18 @@
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -3359,18 +3359,18 @@
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F43" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -3379,18 +3379,18 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3399,18 +3399,18 @@
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F45" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -3422,15 +3422,15 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="F46" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -3439,18 +3439,18 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -3459,23 +3459,23 @@
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -3484,18 +3484,18 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E50" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="F50" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -3504,18 +3504,18 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="F51" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -3527,20 +3527,20 @@
         <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="F52" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -3560,18 +3560,18 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="E55" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -3582,7 +3582,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -3591,18 +3591,18 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F57" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3655,12 +3655,12 @@
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -3669,17 +3669,17 @@
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -3688,21 +3688,21 @@
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="F66" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G66" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -3711,26 +3711,26 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F67" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G67" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3739,18 +3739,18 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E69" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="F69" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -3759,13 +3759,13 @@
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E70" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="F70" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated old and new for obs station to .xyn and .ini. Marked .xyn as supported per 0.5.0.
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HydroLib\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE463E1-2152-4571-8934-12818225F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87CE5DC-9E2D-48C2-B231-9D8FC8BD8CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="167">
   <si>
     <t>Functionality</t>
   </si>
@@ -324,12 +324,6 @@
     <t>**Output**</t>
   </si>
   <si>
-    <t>Observation station file (old)</t>
-  </si>
-  <si>
-    <t>Observation station file (new)</t>
-  </si>
-  <si>
     <t>Observation crosssection file (old)</t>
   </si>
   <si>
@@ -535,6 +529,21 @@
   </si>
   <si>
     <t>hydrolib.core.rr.topology.models</t>
+  </si>
+  <si>
+    <t>Observation station file (.xyn)</t>
+  </si>
+  <si>
+    <t>Observation station file (.ini)</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowm.xyn.models</t>
+  </si>
+  <si>
+    <t>XYNModel</t>
   </si>
 </sst>
 </file>
@@ -2319,23 +2328,23 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
-        <v>Observation station file (old)</v>
+        <v>Observation station file (.xyn)</v>
       </c>
       <c r="B39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C39" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D39" t="str">
         <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.5.0</v>
       </c>
       <c r="E39" t="str">
         <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[XYNModel][hydrolib.core.dflowm.xyn.models.XYNModel]</v>
       </c>
       <c r="F39" t="str">
         <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
@@ -2345,7 +2354,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
-        <v>Observation station file (new)</v>
+        <v>Observation station file (.ini)</v>
       </c>
       <c r="B40" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2586,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,16 +2648,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,7 +2674,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -2685,7 +2694,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
@@ -2702,7 +2711,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,10 +2728,10 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2739,7 +2748,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -2764,7 +2773,7 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -2784,7 +2793,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -2804,7 +2813,7 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
@@ -2824,7 +2833,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F14" t="s">
         <v>38</v>
@@ -2844,7 +2853,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" t="s">
         <v>54</v>
@@ -2864,7 +2873,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
@@ -2895,7 +2904,7 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F18" t="s">
         <v>56</v>
@@ -2915,7 +2924,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
@@ -2935,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -2963,10 +2972,10 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -2986,7 +2995,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
@@ -3006,7 +3015,7 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
         <v>61</v>
@@ -3037,7 +3046,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F26" t="s">
         <v>66</v>
@@ -3057,7 +3066,7 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
         <v>67</v>
@@ -3077,7 +3086,7 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
@@ -3108,7 +3117,7 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F30" t="s">
         <v>70</v>
@@ -3116,7 +3125,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3128,15 +3137,15 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3148,15 +3157,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3168,15 +3177,15 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3185,18 +3194,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3208,15 +3217,15 @@
         <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3228,15 +3237,15 @@
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3245,13 +3254,13 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,7 +3274,7 @@
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3282,7 +3291,7 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F39" t="s">
         <v>73</v>
@@ -3302,7 +3311,7 @@
         <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F40" t="s">
         <v>81</v>
@@ -3322,7 +3331,7 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F41" t="s">
         <v>82</v>
@@ -3342,7 +3351,7 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F42" t="s">
         <v>85</v>
@@ -3362,7 +3371,7 @@
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F43" t="s">
         <v>86</v>
@@ -3382,7 +3391,7 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
@@ -3402,7 +3411,7 @@
         <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F45" t="s">
         <v>84</v>
@@ -3422,7 +3431,7 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F46" t="s">
         <v>72</v>
@@ -3439,10 +3448,10 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F47" t="s">
         <v>88</v>
@@ -3450,32 +3459,32 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>122</v>
       </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>124</v>
-      </c>
       <c r="E48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -3484,18 +3493,18 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -3504,18 +3513,18 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -3527,10 +3536,10 @@
         <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3540,18 +3549,27 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E54" t="s">
+        <v>165</v>
+      </c>
+      <c r="F54" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -3560,18 +3578,18 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -3582,7 +3600,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -3591,18 +3609,18 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E57" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -3613,7 +3631,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -3624,7 +3642,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -3635,7 +3653,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -3646,7 +3664,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3655,12 +3673,12 @@
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -3669,17 +3687,17 @@
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -3691,18 +3709,18 @@
         <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F66" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -3714,23 +3732,23 @@
         <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3739,33 +3757,33 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E69" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F69" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" t="s">
+        <v>161</v>
+      </c>
+      <c r="F70" t="s">
         <v>111</v>
-      </c>
-      <c r="B70" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>124</v>
-      </c>
-      <c r="E70" t="s">
-        <v>163</v>
-      </c>
-      <c r="F70" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated old and new for obs cross section to .pli and .ini. Marked .pli as supported per 0.5.0.
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HydroLib\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87CE5DC-9E2D-48C2-B231-9D8FC8BD8CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417CBAC-C6A0-4CF2-9742-908B695C2025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="169">
   <si>
     <t>Functionality</t>
   </si>
@@ -324,12 +324,6 @@
     <t>**Output**</t>
   </si>
   <si>
-    <t>Observation crosssection file (old)</t>
-  </si>
-  <si>
-    <t>Observation crosssection file (new)</t>
-  </si>
-  <si>
     <t>History file `_his.nc`</t>
   </si>
   <si>
@@ -544,6 +538,18 @@
   </si>
   <si>
     <t>XYNModel</t>
+  </si>
+  <si>
+    <t>Observation crosssection file (.pli)</t>
+  </si>
+  <si>
+    <t>Observation crosssection file (.ini)</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.polyfile.models</t>
+  </si>
+  <si>
+    <t>PolyFile</t>
   </si>
 </sst>
 </file>
@@ -2380,23 +2386,23 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
-        <v>Observation crosssection file (old)</v>
+        <v>Observation crosssection file (.pli)</v>
       </c>
       <c r="B41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C41" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D41" t="str">
         <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.5.0</v>
       </c>
       <c r="E41" t="str">
         <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[PolyFile][hydrolib.core.dflowfm.polyfile.models.PolyFile]</v>
       </c>
       <c r="F41" t="str">
         <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
@@ -2406,7 +2412,7 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
-        <v>Observation crosssection file (new)</v>
+        <v>Observation crosssection file (.ini)</v>
       </c>
       <c r="B42" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
@@ -2596,7 +2602,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,16 +2654,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2674,7 +2680,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -2694,7 +2700,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
@@ -2711,7 +2717,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2728,10 +2734,10 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2748,7 +2754,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -2773,7 +2779,7 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -2793,7 +2799,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -2813,7 +2819,7 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
@@ -2833,7 +2839,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
         <v>38</v>
@@ -2853,7 +2859,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F15" t="s">
         <v>54</v>
@@ -2873,7 +2879,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
@@ -2904,7 +2910,7 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
         <v>56</v>
@@ -2924,7 +2930,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
@@ -2944,7 +2950,7 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -2972,10 +2978,10 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -2995,7 +3001,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
@@ -3015,7 +3021,7 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
         <v>61</v>
@@ -3046,7 +3052,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F26" t="s">
         <v>66</v>
@@ -3066,7 +3072,7 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
         <v>67</v>
@@ -3086,7 +3092,7 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
@@ -3117,7 +3123,7 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F30" t="s">
         <v>70</v>
@@ -3125,7 +3131,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3137,15 +3143,15 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3157,15 +3163,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3177,15 +3183,15 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3194,18 +3200,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3217,15 +3223,15 @@
         <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3237,15 +3243,15 @@
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3254,13 +3260,13 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3274,7 +3280,7 @@
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3291,7 +3297,7 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F39" t="s">
         <v>73</v>
@@ -3311,7 +3317,7 @@
         <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F40" t="s">
         <v>81</v>
@@ -3331,7 +3337,7 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
         <v>82</v>
@@ -3351,7 +3357,7 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F42" t="s">
         <v>85</v>
@@ -3371,7 +3377,7 @@
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F43" t="s">
         <v>86</v>
@@ -3391,7 +3397,7 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
@@ -3411,7 +3417,7 @@
         <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F45" t="s">
         <v>84</v>
@@ -3431,7 +3437,7 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F46" t="s">
         <v>72</v>
@@ -3448,10 +3454,10 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F47" t="s">
         <v>88</v>
@@ -3459,32 +3465,32 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
         <v>120</v>
       </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>122</v>
-      </c>
       <c r="E48" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -3493,18 +3499,18 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -3513,18 +3519,18 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -3536,10 +3542,10 @@
         <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3549,27 +3555,27 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
         <v>162</v>
       </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" t="s">
         <v>164</v>
-      </c>
-      <c r="E54" t="s">
-        <v>165</v>
-      </c>
-      <c r="F54" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -3578,29 +3584,38 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>162</v>
+      </c>
+      <c r="E56" t="s">
+        <v>167</v>
+      </c>
+      <c r="F56" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -3609,18 +3624,18 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -3631,7 +3646,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -3642,7 +3657,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -3653,7 +3668,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -3664,7 +3679,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3673,12 +3688,12 @@
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -3687,17 +3702,17 @@
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -3709,18 +3724,18 @@
         <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F66" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -3732,23 +3747,23 @@
         <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F67" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3757,33 +3772,33 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>107</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" t="s">
+        <v>159</v>
+      </c>
+      <c r="F70" t="s">
         <v>109</v>
-      </c>
-      <c r="B70" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>122</v>
-      </c>
-      <c r="E70" t="s">
-        <v>161</v>
-      </c>
-      <c r="F70" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the ext file entries
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HydroLib\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417CBAC-C6A0-4CF2-9742-908B695C2025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EC608A-5514-4FCB-902A-7C38AAD8AFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$A$1:$G$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="175">
   <si>
     <t>Functionality</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Lateral</t>
   </si>
   <si>
-    <t>* .bc file</t>
-  </si>
-  <si>
     <t>ForcingModel</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>**Cross section files**</t>
   </si>
   <si>
-    <t>**External forcings file (new)**</t>
-  </si>
-  <si>
     <t>**Output**</t>
   </si>
   <si>
@@ -426,27 +420,6 @@
     <t>Used to be in hydrolib.core.io.bui.models before 0.3.0</t>
   </si>
   <si>
-    <t>** timeSeries</t>
-  </si>
-  <si>
-    <t>** harmonic (-Correction)</t>
-  </si>
-  <si>
-    <t>** astronomic (-Correction)</t>
-  </si>
-  <si>
-    <t>** t3D</t>
-  </si>
-  <si>
-    <t>** QHTable</t>
-  </si>
-  <si>
-    <t>** constant</t>
-  </si>
-  <si>
-    <t>** vector quantities</t>
-  </si>
-  <si>
     <t>TimeSeries</t>
   </si>
   <si>
@@ -550,6 +523,51 @@
   </si>
   <si>
     <t>PolyFile</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.extold.models</t>
+  </si>
+  <si>
+    <t>ExtOldModel</t>
+  </si>
+  <si>
+    <t>**External forcings file**</t>
+  </si>
+  <si>
+    <t>External forcings file (new)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .bc file</t>
+  </si>
+  <si>
+    <t>* timeSeries</t>
+  </si>
+  <si>
+    <t>* harmonic (-Correction)</t>
+  </si>
+  <si>
+    <t>* astronomic (-Correction)</t>
+  </si>
+  <si>
+    <t>* t3D</t>
+  </si>
+  <si>
+    <t>* QHTable</t>
+  </si>
+  <si>
+    <t>* constant</t>
+  </si>
+  <si>
+    <t>* vector quantities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .tim file</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.tim.models</t>
+  </si>
+  <si>
+    <t>TimModel</t>
   </si>
 </sst>
 </file>
@@ -1173,157 +1191,157 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>IF(ISBLANK('Source table'!A65)," ",'Source table'!A65)</f>
+        <f>IF(ISBLANK('Source table'!A67)," ",'Source table'!A67)</f>
         <v>**RR**</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISBLANK('Source table'!D65)," ",'Source table'!D65)</f>
+        <f>IF(ISBLANK('Source table'!D67)," ",'Source table'!D67)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E2" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E65),ISBLANK('Source table'!F65))," ","["&amp;'Source table'!F65&amp;"]["&amp;'Source table'!E65&amp;"."&amp;'Source table'!F65&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" t="str">
-        <f>IF(ISBLANK('Source table'!G65)," ","_"&amp;'Source table'!G65&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>IF(ISBLANK('Source table'!A66)," ",'Source table'!A66)</f>
+        <f>IF(ISBLANK('Source table'!A68)," ",'Source table'!A68)</f>
         <v>Main sobek_3b.fnm</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C66,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(ISBLANK('Source table'!D66)," ",'Source table'!D66)</f>
+        <f>IF(ISBLANK('Source table'!D68)," ",'Source table'!D68)</f>
         <v>0.1.5</v>
       </c>
       <c r="E3" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E66),ISBLANK('Source table'!F66))," ","["&amp;'Source table'!F66&amp;"]["&amp;'Source table'!E66&amp;"."&amp;'Source table'!F66&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E68),ISBLANK('Source table'!F68))," ","["&amp;'Source table'!F68&amp;"]["&amp;'Source table'!E68&amp;"."&amp;'Source table'!F68&amp;"]")</f>
         <v>[RainfallRunoffModel][hydrolib.core.rr.models.RainfallRunoffModel]</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(ISBLANK('Source table'!G66)," ","_"&amp;'Source table'!G66&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G68)," ","_"&amp;'Source table'!G68&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.fnm.models before 0.3.0_</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>IF(ISBLANK('Source table'!A67)," ",'Source table'!A67)</f>
+        <f>IF(ISBLANK('Source table'!A69)," ",'Source table'!A69)</f>
         <v>Rainfall .bui file</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C67,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(ISBLANK('Source table'!D67)," ",'Source table'!D67)</f>
+        <f>IF(ISBLANK('Source table'!D69)," ",'Source table'!D69)</f>
         <v>0.1.5</v>
       </c>
       <c r="E4" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E67),ISBLANK('Source table'!F67))," ","["&amp;'Source table'!F67&amp;"]["&amp;'Source table'!E67&amp;"."&amp;'Source table'!F67&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
         <v>[BuiModel][hydrolib.core.rr.meteo.models.BuiModel]</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(ISBLANK('Source table'!G67)," ","_"&amp;'Source table'!G67&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
         <v>_Used to be in hydrolib.core.io.bui.models before 0.3.0_</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>IF(ISBLANK('Source table'!A68)," ",'Source table'!A68)</f>
+        <f>IF(ISBLANK('Source table'!A70)," ",'Source table'!A70)</f>
         <v>**Topology layer**</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C68,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK('Source table'!D68)," ",'Source table'!D68)</f>
+        <f>IF(ISBLANK('Source table'!D70)," ",'Source table'!D70)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E5" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E68),ISBLANK('Source table'!F68))," ","["&amp;'Source table'!F68&amp;"]["&amp;'Source table'!E68&amp;"."&amp;'Source table'!F68&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" t="str">
-        <f>IF(ISBLANK('Source table'!G68)," ","_"&amp;'Source table'!G68&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>IF(ISBLANK('Source table'!A69)," ",'Source table'!A69)</f>
+        <f>IF(ISBLANK('Source table'!A71)," ",'Source table'!A71)</f>
         <v>Node file 3b_node.tp</v>
       </c>
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B71,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C69,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C71,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(ISBLANK('Source table'!D69)," ",'Source table'!D69)</f>
+        <f>IF(ISBLANK('Source table'!D71)," ",'Source table'!D71)</f>
         <v>0.2.0</v>
       </c>
       <c r="E6" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E69),ISBLANK('Source table'!F69))," ","["&amp;'Source table'!F69&amp;"]["&amp;'Source table'!E69&amp;"."&amp;'Source table'!F69&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E71),ISBLANK('Source table'!F71))," ","["&amp;'Source table'!F71&amp;"]["&amp;'Source table'!E71&amp;"."&amp;'Source table'!F71&amp;"]")</f>
         <v>[NodeFile][hydrolib.core.rr.topology.models.NodeFile]</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(ISBLANK('Source table'!G69)," ","_"&amp;'Source table'!G69&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G71)," ","_"&amp;'Source table'!G71&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>IF(ISBLANK('Source table'!A70)," ",'Source table'!A70)</f>
+        <f>IF(ISBLANK('Source table'!A72)," ",'Source table'!A72)</f>
         <v>Link file 3b_link.tp</v>
       </c>
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B72,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C70,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C72,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(ISBLANK('Source table'!D70)," ",'Source table'!D70)</f>
+        <f>IF(ISBLANK('Source table'!D72)," ",'Source table'!D72)</f>
         <v>0.2.0</v>
       </c>
       <c r="E7" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E70),ISBLANK('Source table'!F70))," ","["&amp;'Source table'!F70&amp;"]["&amp;'Source table'!E70&amp;"."&amp;'Source table'!F70&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E72),ISBLANK('Source table'!F72))," ","["&amp;'Source table'!F72&amp;"]["&amp;'Source table'!E72&amp;"."&amp;'Source table'!F72&amp;"]")</f>
         <v>[LinkFile][hydrolib.core.rr.topology.models.LinkFile]</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(ISBLANK('Source table'!G70)," ","_"&amp;'Source table'!G70&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G72)," ","_"&amp;'Source table'!G72&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1337,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A9C44C-39DD-AE4F-8193-56F00A265DD6}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,23 +1780,23 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(ISBLANK('Source table'!A25)," ",'Source table'!A25)</f>
-        <v>External forcings file (old)</v>
+        <v>**External forcings file**</v>
       </c>
       <c r="B17" t="str">
         <f>IFERROR(VLOOKUP('Source table'!B25,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C17" t="str">
         <f>IFERROR(VLOOKUP('Source table'!C25,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
-        <v>:x:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK('Source table'!D25)," ",'Source table'!D25)</f>
-        <v xml:space="preserve"> </v>
+        <v>0.5.0</v>
       </c>
       <c r="E17" t="str">
         <f>IF(OR(ISBLANK('Source table'!E25),ISBLANK('Source table'!F25))," ","["&amp;'Source table'!F25&amp;"]["&amp;'Source table'!E25&amp;"."&amp;'Source table'!F25&amp;"]")</f>
-        <v xml:space="preserve"> </v>
+        <v>[ExtOldModel][hydrolib.core.dflowfm.extold.models.ExtOldModel]</v>
       </c>
       <c r="F17" t="str">
         <f>IF(ISBLANK('Source table'!G25)," ","_"&amp;'Source table'!G25&amp;"_")</f>
@@ -1787,807 +1805,807 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>IF(ISBLANK('Source table'!A26)," ",'Source table'!A26)</f>
-        <v>**External forcings file (new)**</v>
+        <f>IF(ISBLANK('Source table'!A27)," ",'Source table'!A27)</f>
+        <v>External forcings file (new)</v>
       </c>
       <c r="B18" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B26,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B27,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C18" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C26,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C27,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D18" t="str">
-        <f>IF(ISBLANK('Source table'!D26)," ",'Source table'!D26)</f>
+        <f>IF(ISBLANK('Source table'!D27)," ",'Source table'!D27)</f>
         <v>0.1.1</v>
       </c>
       <c r="E18" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E26),ISBLANK('Source table'!F26))," ","["&amp;'Source table'!F26&amp;"]["&amp;'Source table'!E26&amp;"."&amp;'Source table'!F26&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E27),ISBLANK('Source table'!F27))," ","["&amp;'Source table'!F27&amp;"]["&amp;'Source table'!E27&amp;"."&amp;'Source table'!F27&amp;"]")</f>
         <v>[ExtModel][hydrolib.core.dflowfm.ext.models.ExtModel]</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(ISBLANK('Source table'!G26)," ","_"&amp;'Source table'!G26&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G27)," ","_"&amp;'Source table'!G27&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>IF(ISBLANK('Source table'!A27)," ",'Source table'!A27)</f>
+        <f>IF(ISBLANK('Source table'!A28)," ",'Source table'!A28)</f>
         <v>* Boundary</v>
       </c>
       <c r="B19" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B27,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B28,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C19" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C27,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C28,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D19" t="str">
-        <f>IF(ISBLANK('Source table'!D27)," ",'Source table'!D27)</f>
+        <f>IF(ISBLANK('Source table'!D28)," ",'Source table'!D28)</f>
         <v>0.1.1</v>
       </c>
       <c r="E19" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E27),ISBLANK('Source table'!F27))," ","["&amp;'Source table'!F27&amp;"]["&amp;'Source table'!E27&amp;"."&amp;'Source table'!F27&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E28),ISBLANK('Source table'!F28))," ","["&amp;'Source table'!F28&amp;"]["&amp;'Source table'!E28&amp;"."&amp;'Source table'!F28&amp;"]")</f>
         <v>[Boundary][hydrolib.core.dflowfm.ext.models.Boundary]</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(ISBLANK('Source table'!G27)," ","_"&amp;'Source table'!G27&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G28)," ","_"&amp;'Source table'!G28&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>IF(ISBLANK('Source table'!A28)," ",'Source table'!A28)</f>
+        <f>IF(ISBLANK('Source table'!A29)," ",'Source table'!A29)</f>
         <v>* Lateral</v>
       </c>
       <c r="B20" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B28,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B29,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C20" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C28,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C29,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D20" t="str">
-        <f>IF(ISBLANK('Source table'!D28)," ",'Source table'!D28)</f>
+        <f>IF(ISBLANK('Source table'!D29)," ",'Source table'!D29)</f>
         <v>0.1.1</v>
       </c>
       <c r="E20" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E28),ISBLANK('Source table'!F28))," ","["&amp;'Source table'!F28&amp;"]["&amp;'Source table'!E28&amp;"."&amp;'Source table'!F28&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E29),ISBLANK('Source table'!F29))," ","["&amp;'Source table'!F29&amp;"]["&amp;'Source table'!E29&amp;"."&amp;'Source table'!F29&amp;"]")</f>
         <v>[Lateral][hydrolib.core.dflowfm.ext.models.Lateral]</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(ISBLANK('Source table'!G28)," ","_"&amp;'Source table'!G28&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G29)," ","_"&amp;'Source table'!G29&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>IF(ISBLANK('Source table'!A29)," ",'Source table'!A29)</f>
+        <f>IF(ISBLANK('Source table'!A30)," ",'Source table'!A30)</f>
         <v>* Meteo</v>
       </c>
       <c r="B21" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B29,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B30,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C21" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C29,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C30,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D21" t="str">
-        <f>IF(ISBLANK('Source table'!D29)," ",'Source table'!D29)</f>
+        <f>IF(ISBLANK('Source table'!D30)," ",'Source table'!D30)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E21" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E29),ISBLANK('Source table'!F29))," ","["&amp;'Source table'!F29&amp;"]["&amp;'Source table'!E29&amp;"."&amp;'Source table'!F29&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E30),ISBLANK('Source table'!F30))," ","["&amp;'Source table'!F30&amp;"]["&amp;'Source table'!E30&amp;"."&amp;'Source table'!F30&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F21" t="str">
-        <f>IF(ISBLANK('Source table'!G29)," ","_"&amp;'Source table'!G29&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G30)," ","_"&amp;'Source table'!G30&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>IF(ISBLANK('Source table'!A30)," ",'Source table'!A30)</f>
-        <v>* .bc file</v>
+        <f>IF(ISBLANK('Source table'!A31)," ",'Source table'!A31)</f>
+        <v xml:space="preserve"> .bc file</v>
       </c>
       <c r="B22" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B30,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C22" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C30,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C31,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D22" t="str">
-        <f>IF(ISBLANK('Source table'!D30)," ",'Source table'!D30)</f>
+        <f>IF(ISBLANK('Source table'!D31)," ",'Source table'!D31)</f>
         <v>0.1.1</v>
       </c>
       <c r="E22" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E30),ISBLANK('Source table'!F30))," ","["&amp;'Source table'!F30&amp;"]["&amp;'Source table'!E30&amp;"."&amp;'Source table'!F30&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E31),ISBLANK('Source table'!F31))," ","["&amp;'Source table'!F31&amp;"]["&amp;'Source table'!E31&amp;"."&amp;'Source table'!F31&amp;"]")</f>
         <v>[ForcingModel][hydrolib.core.dflowfm.bc.models.ForcingModel]</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(ISBLANK('Source table'!G30)," ","_"&amp;'Source table'!G30&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G31)," ","_"&amp;'Source table'!G31&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>IF(ISBLANK('Source table'!A38)," ",'Source table'!A38)</f>
+        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
         <v>**Cross section files**</v>
       </c>
       <c r="B23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C23" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C38,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D23" t="str">
-        <f>IF(ISBLANK('Source table'!D38)," ",'Source table'!D38)</f>
+        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E23" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E38),ISBLANK('Source table'!F38))," ","["&amp;'Source table'!F38&amp;"]["&amp;'Source table'!E38&amp;"."&amp;'Source table'!F38&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F23" t="str">
-        <f>IF(ISBLANK('Source table'!G38)," ","_"&amp;'Source table'!G38&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
         <v>_Moved to io.crosssections in 0.2.0_</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>IF(ISBLANK('Source table'!A39)," ",'Source table'!A39)</f>
+        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
         <v>Cross section definition file</v>
       </c>
       <c r="B24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C24" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C39,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D24" t="str">
-        <f>IF(ISBLANK('Source table'!D39)," ",'Source table'!D39)</f>
+        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
         <v>0.1.1</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E39),ISBLANK('Source table'!F39))," ","["&amp;'Source table'!F39&amp;"]["&amp;'Source table'!E39&amp;"."&amp;'Source table'!F39&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
         <v>[CrossDefModel][hydrolib.core.dflowfm.crosssection.models.CrossDefModel]</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(ISBLANK('Source table'!G39)," ","_"&amp;'Source table'!G39&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>IF(ISBLANK('Source table'!A40)," ",'Source table'!A40)</f>
+        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
         <v>* Circle</v>
       </c>
       <c r="B25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C25" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C40,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D25" t="str">
-        <f>IF(ISBLANK('Source table'!D40)," ",'Source table'!D40)</f>
+        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
         <v>0.1.5</v>
       </c>
       <c r="E25" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E40),ISBLANK('Source table'!F40))," ","["&amp;'Source table'!F40&amp;"]["&amp;'Source table'!E40&amp;"."&amp;'Source table'!F40&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
         <v>[CircleCrsDef][hydrolib.core.dflowfm.crosssection.models.CircleCrsDef]</v>
       </c>
       <c r="F25" t="str">
-        <f>IF(ISBLANK('Source table'!G40)," ","_"&amp;'Source table'!G40&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>IF(ISBLANK('Source table'!A41)," ",'Source table'!A41)</f>
+        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
         <v>* Rectangle</v>
       </c>
       <c r="B26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C26" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C41,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D26" t="str">
-        <f>IF(ISBLANK('Source table'!D41)," ",'Source table'!D41)</f>
+        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
         <v>0.1.5</v>
       </c>
       <c r="E26" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E41),ISBLANK('Source table'!F41))," ","["&amp;'Source table'!F41&amp;"]["&amp;'Source table'!E41&amp;"."&amp;'Source table'!F41&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
         <v>[RectangleCrsDef][hydrolib.core.dflowfm.crosssection.models.RectangleCrsDef]</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(ISBLANK('Source table'!G41)," ","_"&amp;'Source table'!G41&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>IF(ISBLANK('Source table'!A42)," ",'Source table'!A42)</f>
+        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
         <v>* Tabulated river</v>
       </c>
       <c r="B27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C27" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C42,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D27" t="str">
-        <f>IF(ISBLANK('Source table'!D42)," ",'Source table'!D42)</f>
+        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
         <v>0.1.5</v>
       </c>
       <c r="E27" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E42),ISBLANK('Source table'!F42))," ","["&amp;'Source table'!F42&amp;"]["&amp;'Source table'!E42&amp;"."&amp;'Source table'!F42&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
         <v>[ZWRiverCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWRiverCrsDef]</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(ISBLANK('Source table'!G42)," ","_"&amp;'Source table'!G42&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>IF(ISBLANK('Source table'!A43)," ",'Source table'!A43)</f>
+        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
         <v>* ZW (tabulated)</v>
       </c>
       <c r="B28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C28" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C43,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D28" t="str">
-        <f>IF(ISBLANK('Source table'!D43)," ",'Source table'!D43)</f>
+        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
         <v>0.1.5</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E43),ISBLANK('Source table'!F43))," ","["&amp;'Source table'!F43&amp;"]["&amp;'Source table'!E43&amp;"."&amp;'Source table'!F43&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
         <v>[ZWCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWCrsDef]</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(ISBLANK('Source table'!G43)," ","_"&amp;'Source table'!G43&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>IF(ISBLANK('Source table'!A44)," ",'Source table'!A44)</f>
+        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
         <v>* XYZ</v>
       </c>
       <c r="B29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C29" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C44,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D29" t="str">
-        <f>IF(ISBLANK('Source table'!D44)," ",'Source table'!D44)</f>
+        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
         <v>0.1.5</v>
       </c>
       <c r="E29" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E44),ISBLANK('Source table'!F44))," ","["&amp;'Source table'!F44&amp;"]["&amp;'Source table'!E44&amp;"."&amp;'Source table'!F44&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
         <v>[XYZCrsDef][hydrolib.core.dflowfm.crosssection.models.XYZCrsDef]</v>
       </c>
       <c r="F29" t="str">
-        <f>IF(ISBLANK('Source table'!G44)," ","_"&amp;'Source table'!G44&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>IF(ISBLANK('Source table'!A45)," ",'Source table'!A45)</f>
+        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
         <v>* YZ</v>
       </c>
       <c r="B30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C30" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C45,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D30" t="str">
-        <f>IF(ISBLANK('Source table'!D45)," ",'Source table'!D45)</f>
+        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
         <v>0.1.5</v>
       </c>
       <c r="E30" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E45),ISBLANK('Source table'!F45))," ","["&amp;'Source table'!F45&amp;"]["&amp;'Source table'!E45&amp;"."&amp;'Source table'!F45&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
         <v>[YZCrsDef][hydrolib.core.dflowfm.crosssection.models.YZCrsDef]</v>
       </c>
       <c r="F30" t="str">
-        <f>IF(ISBLANK('Source table'!G45)," ","_"&amp;'Source table'!G45&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>IF(ISBLANK('Source table'!A46)," ",'Source table'!A46)</f>
+        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
         <v>Cross section location file</v>
       </c>
       <c r="B31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C31" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C46,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D31" t="str">
-        <f>IF(ISBLANK('Source table'!D46)," ",'Source table'!D46)</f>
+        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
         <v>0.1.1</v>
       </c>
       <c r="E31" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E46),ISBLANK('Source table'!F46))," ","["&amp;'Source table'!F46&amp;"]["&amp;'Source table'!E46&amp;"."&amp;'Source table'!F46&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
         <v>[CrossLocModel][hydrolib.core.dflowfm.crosssection.models.CrossLocModel]</v>
       </c>
       <c r="F31" t="str">
-        <f>IF(ISBLANK('Source table'!G46)," ","_"&amp;'Source table'!G46&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>IF(ISBLANK('Source table'!A47)," ",'Source table'!A47)</f>
+        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
         <v>1D roughness file</v>
       </c>
       <c r="B32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C32" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C47,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D32" t="str">
-        <f>IF(ISBLANK('Source table'!D47)," ",'Source table'!D47)</f>
+        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
         <v>0.2.0</v>
       </c>
       <c r="E32" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E47),ISBLANK('Source table'!F47))," ","["&amp;'Source table'!F47&amp;"]["&amp;'Source table'!E47&amp;"."&amp;'Source table'!F47&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
         <v>[FrictionModel][hydrolib.core.dflowfm.friction.models.FrictionModel]</v>
       </c>
       <c r="F32" t="str">
-        <f>IF(ISBLANK('Source table'!G47)," ","_"&amp;'Source table'!G47&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>IF(ISBLANK('Source table'!A48)," ",'Source table'!A48)</f>
+        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
         <v>Storage node file</v>
       </c>
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C33" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C48,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D33" t="str">
-        <f>IF(ISBLANK('Source table'!D48)," ",'Source table'!D48)</f>
+        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
         <v>0.2.0</v>
       </c>
       <c r="E33" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E48),ISBLANK('Source table'!F48))," ","["&amp;'Source table'!F48&amp;"]["&amp;'Source table'!E48&amp;"."&amp;'Source table'!F48&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
         <v>[StorageNodeModel][hydrolib.core.dflowfm.storagenode.models.StorageNodeModel]</v>
       </c>
       <c r="F33" t="str">
-        <f>IF(ISBLANK('Source table'!G48)," ","_"&amp;'Source table'!G48&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>IF(ISBLANK('Source table'!A49)," ",'Source table'!A49)</f>
+        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
         <v>**Spatial data files**</v>
       </c>
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C34" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C49,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D34" t="str">
-        <f>IF(ISBLANK('Source table'!D49)," ",'Source table'!D49)</f>
+        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E34" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E49),ISBLANK('Source table'!F49))," ","["&amp;'Source table'!F49&amp;"]["&amp;'Source table'!E49&amp;"."&amp;'Source table'!F49&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F34" t="str">
-        <f>IF(ISBLANK('Source table'!G49)," ","_"&amp;'Source table'!G49&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>IF(ISBLANK('Source table'!A50)," ",'Source table'!A50)</f>
+        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
         <v>Initial and parameter field file</v>
       </c>
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C35" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C50,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D35" t="str">
-        <f>IF(ISBLANK('Source table'!D50)," ",'Source table'!D50)</f>
+        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
         <v>0.2.0</v>
       </c>
       <c r="E35" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E50),ISBLANK('Source table'!F50))," ","["&amp;'Source table'!F50&amp;"]["&amp;'Source table'!E50&amp;"."&amp;'Source table'!F50&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
         <v>[IniFieldModel][hydrolib.core.dflowfm.inifield.models.IniFieldModel]</v>
       </c>
       <c r="F35" t="str">
-        <f>IF(ISBLANK('Source table'!G50)," ","_"&amp;'Source table'!G50&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>IF(ISBLANK('Source table'!A51)," ",'Source table'!A51)</f>
+        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
         <v>1D field INI files</v>
       </c>
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C36" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C51,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D36" t="str">
-        <f>IF(ISBLANK('Source table'!D51)," ",'Source table'!D51)</f>
+        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
         <v>0.2.0</v>
       </c>
       <c r="E36" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E51),ISBLANK('Source table'!F51))," ","["&amp;'Source table'!F51&amp;"]["&amp;'Source table'!E51&amp;"."&amp;'Source table'!F51&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
         <v>[OneDFieldModel][hydrolib.core.dflowfm.onedfield.models.OneDFieldModel]</v>
       </c>
       <c r="F36" t="str">
-        <f>IF(ISBLANK('Source table'!G51)," ","_"&amp;'Source table'!G51&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>IF(ISBLANK('Source table'!A52)," ",'Source table'!A52)</f>
+        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
         <v>Sample file</v>
       </c>
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C37" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C52,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D37" t="str">
-        <f>IF(ISBLANK('Source table'!D52)," ",'Source table'!D52)</f>
+        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
         <v>0.1.1</v>
       </c>
       <c r="E37" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E52),ISBLANK('Source table'!F52))," ","["&amp;'Source table'!F52&amp;"]["&amp;'Source table'!E52&amp;"."&amp;'Source table'!F52&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
         <v>[XYZModel][hydrolib.core.dflowfm.xyz.models.XYZModel]</v>
       </c>
       <c r="F37" t="str">
-        <f>IF(ISBLANK('Source table'!G52)," ","_"&amp;'Source table'!G52&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>IF(ISBLANK('Source table'!A53)," ",'Source table'!A53)</f>
+        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
         <v>**Output**</v>
       </c>
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C38" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C53,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D38" t="str">
-        <f>IF(ISBLANK('Source table'!D53)," ",'Source table'!D53)</f>
+        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E38" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E53),ISBLANK('Source table'!F53))," ","["&amp;'Source table'!F53&amp;"]["&amp;'Source table'!E53&amp;"."&amp;'Source table'!F53&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" t="str">
-        <f>IF(ISBLANK('Source table'!G53)," ","_"&amp;'Source table'!G53&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>IF(ISBLANK('Source table'!A54)," ",'Source table'!A54)</f>
+        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
         <v>Observation station file (.xyn)</v>
       </c>
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C39" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C54,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D39" t="str">
-        <f>IF(ISBLANK('Source table'!D54)," ",'Source table'!D54)</f>
+        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
         <v>0.5.0</v>
       </c>
       <c r="E39" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E54),ISBLANK('Source table'!F54))," ","["&amp;'Source table'!F54&amp;"]["&amp;'Source table'!E54&amp;"."&amp;'Source table'!F54&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
         <v>[XYNModel][hydrolib.core.dflowm.xyn.models.XYNModel]</v>
       </c>
       <c r="F39" t="str">
-        <f>IF(ISBLANK('Source table'!G54)," ","_"&amp;'Source table'!G54&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>IF(ISBLANK('Source table'!A55)," ",'Source table'!A55)</f>
+        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
         <v>Observation station file (.ini)</v>
       </c>
       <c r="B40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C40" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C55,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D40" t="str">
-        <f>IF(ISBLANK('Source table'!D55)," ",'Source table'!D55)</f>
+        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
         <v>0.3.0</v>
       </c>
       <c r="E40" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E55),ISBLANK('Source table'!F55))," ","["&amp;'Source table'!F55&amp;"]["&amp;'Source table'!E55&amp;"."&amp;'Source table'!F55&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
         <v>[ObservationPointModel][hydrolib.core.dflowfm.obs.models.ObservationPointModel]</v>
       </c>
       <c r="F40" t="str">
-        <f>IF(ISBLANK('Source table'!G55)," ","_"&amp;'Source table'!G55&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>IF(ISBLANK('Source table'!A56)," ",'Source table'!A56)</f>
+        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
         <v>Observation crosssection file (.pli)</v>
       </c>
       <c r="B41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C41" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C56,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D41" t="str">
-        <f>IF(ISBLANK('Source table'!D56)," ",'Source table'!D56)</f>
+        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
         <v>0.5.0</v>
       </c>
       <c r="E41" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E56),ISBLANK('Source table'!F56))," ","["&amp;'Source table'!F56&amp;"]["&amp;'Source table'!E56&amp;"."&amp;'Source table'!F56&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
         <v>[PolyFile][hydrolib.core.dflowfm.polyfile.models.PolyFile]</v>
       </c>
       <c r="F41" t="str">
-        <f>IF(ISBLANK('Source table'!G56)," ","_"&amp;'Source table'!G56&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>IF(ISBLANK('Source table'!A57)," ",'Source table'!A57)</f>
+        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
         <v>Observation crosssection file (.ini)</v>
       </c>
       <c r="B42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="C42" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C57,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:white_check_mark:</v>
       </c>
       <c r="D42" t="str">
-        <f>IF(ISBLANK('Source table'!D57)," ",'Source table'!D57)</f>
+        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
         <v>0.3.1</v>
       </c>
       <c r="E42" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E57),ISBLANK('Source table'!F57))," ","["&amp;'Source table'!F57&amp;"]["&amp;'Source table'!E57&amp;"."&amp;'Source table'!F57&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
         <v>[ObservationCrossSectionModel][hydrolib.core.dflowfm.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
       <c r="F42" t="str">
-        <f>IF(ISBLANK('Source table'!G57)," ","_"&amp;'Source table'!G57&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>IF(ISBLANK('Source table'!A58)," ",'Source table'!A58)</f>
+        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
         <v>History file `_his.nc`</v>
       </c>
       <c r="B43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C43" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C58,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D43" t="str">
-        <f>IF(ISBLANK('Source table'!D58)," ",'Source table'!D58)</f>
+        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E58),ISBLANK('Source table'!F58))," ","["&amp;'Source table'!F58&amp;"]["&amp;'Source table'!E58&amp;"."&amp;'Source table'!F58&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" t="str">
-        <f>IF(ISBLANK('Source table'!G58)," ","_"&amp;'Source table'!G58&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>IF(ISBLANK('Source table'!A59)," ",'Source table'!A59)</f>
+        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
         <v>Map file (old)</v>
       </c>
       <c r="B44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C44" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C59,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D44" t="str">
-        <f>IF(ISBLANK('Source table'!D59)," ",'Source table'!D59)</f>
+        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E59),ISBLANK('Source table'!F59))," ","["&amp;'Source table'!F59&amp;"]["&amp;'Source table'!E59&amp;"."&amp;'Source table'!F59&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F44" t="str">
-        <f>IF(ISBLANK('Source table'!G59)," ","_"&amp;'Source table'!G59&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>IF(ISBLANK('Source table'!A60)," ",'Source table'!A60)</f>
+        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
       <c r="B45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C45" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C60,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D45" t="str">
-        <f>IF(ISBLANK('Source table'!D60)," ",'Source table'!D60)</f>
+        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E60),ISBLANK('Source table'!F60))," ","["&amp;'Source table'!F60&amp;"]["&amp;'Source table'!E60&amp;"."&amp;'Source table'!F60&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F45" t="str">
-        <f>IF(ISBLANK('Source table'!G60)," ","_"&amp;'Source table'!G60&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>IF(ISBLANK('Source table'!A61)," ",'Source table'!A61)</f>
+        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
         <v>Fourier input file</v>
       </c>
       <c r="B46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="C46" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C61,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:x:</v>
       </c>
       <c r="D46" t="str">
-        <f>IF(ISBLANK('Source table'!D61)," ",'Source table'!D61)</f>
+        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E61),ISBLANK('Source table'!F61))," ","["&amp;'Source table'!F61&amp;"]["&amp;'Source table'!E61&amp;"."&amp;'Source table'!F61&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F46" t="str">
-        <f>IF(ISBLANK('Source table'!G61)," ","_"&amp;'Source table'!G61&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>IF(ISBLANK('Source table'!A62)," ",'Source table'!A62)</f>
+        <f>IF(ISBLANK('Source table'!A64)," ",'Source table'!A64)</f>
         <v>Fourier output file `_fou.nc`</v>
       </c>
       <c r="B47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B64,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C47" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C62,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C64,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D47" t="str">
-        <f>IF(ISBLANK('Source table'!D62)," ",'Source table'!D62)</f>
+        <f>IF(ISBLANK('Source table'!D64)," ",'Source table'!D64)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E47" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E62),ISBLANK('Source table'!F62))," ","["&amp;'Source table'!F62&amp;"]["&amp;'Source table'!E62&amp;"."&amp;'Source table'!F62&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E64),ISBLANK('Source table'!F64))," ","["&amp;'Source table'!F64&amp;"]["&amp;'Source table'!E64&amp;"."&amp;'Source table'!F64&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F47" t="str">
-        <f>IF(ISBLANK('Source table'!G62)," ","_"&amp;'Source table'!G62&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G64)," ","_"&amp;'Source table'!G64&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>IF(ISBLANK('Source table'!A63)," ",'Source table'!A63)</f>
+        <f>IF(ISBLANK('Source table'!A65)," ",'Source table'!A65)</f>
         <v>Class map file</v>
       </c>
       <c r="B48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!B63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!B65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="C48" t="str">
-        <f>IFERROR(VLOOKUP('Source table'!C63,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
+        <f>IFERROR(VLOOKUP('Source table'!C65,'mkdocs symbols'!$A$1:$C$5,2,0)," ")</f>
         <v>:material-close-box:</v>
       </c>
       <c r="D48" t="str">
-        <f>IF(ISBLANK('Source table'!D63)," ",'Source table'!D63)</f>
+        <f>IF(ISBLANK('Source table'!D65)," ",'Source table'!D65)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E48" t="str">
-        <f>IF(OR(ISBLANK('Source table'!E63),ISBLANK('Source table'!F63))," ","["&amp;'Source table'!F63&amp;"]["&amp;'Source table'!E63&amp;"."&amp;'Source table'!F63&amp;"]")</f>
+        <f>IF(OR(ISBLANK('Source table'!E65),ISBLANK('Source table'!F65))," ","["&amp;'Source table'!F65&amp;"]["&amp;'Source table'!E65&amp;"."&amp;'Source table'!F65&amp;"]")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F48" t="str">
-        <f>IF(ISBLANK('Source table'!G63)," ","_"&amp;'Source table'!G63&amp;"_")</f>
+        <f>IF(ISBLANK('Source table'!G65)," ","_"&amp;'Source table'!G65&amp;"_")</f>
         <v>_via map file reader_</v>
       </c>
     </row>
@@ -2599,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2628,7 @@
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2654,16 +2672,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2680,7 +2698,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -2700,7 +2718,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
@@ -2717,7 +2735,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2734,10 +2752,10 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2754,7 +2772,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -2779,7 +2797,7 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -2799,7 +2817,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
         <v>40</v>
@@ -2807,7 +2825,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -2819,7 +2837,7 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
@@ -2839,7 +2857,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
         <v>38</v>
@@ -2859,7 +2877,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F15" t="s">
         <v>54</v>
@@ -2879,7 +2897,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
@@ -2910,7 +2928,7 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F18" t="s">
         <v>56</v>
@@ -2930,7 +2948,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F19" t="s">
         <v>57</v>
@@ -2950,7 +2968,7 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -2978,10 +2996,10 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
@@ -3001,7 +3019,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
@@ -3021,7 +3039,7 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F24" t="s">
         <v>61</v>
@@ -3029,38 +3047,32 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3072,15 +3084,15 @@
         <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3092,46 +3104,46 @@
         <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3143,15 +3155,15 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3163,15 +3175,15 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -3183,15 +3195,15 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -3200,18 +3212,18 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -3220,18 +3232,18 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -3243,15 +3255,15 @@
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F36" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -3260,18 +3272,18 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F37" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -3279,13 +3291,19 @@
       <c r="C38" t="s">
         <v>10</v>
       </c>
-      <c r="G38" t="s">
-        <v>121</v>
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3294,18 +3312,18 @@
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="F39" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -3313,19 +3331,13 @@
       <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="D40" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" t="s">
-        <v>149</v>
-      </c>
-      <c r="F40" t="s">
-        <v>81</v>
+      <c r="G40" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -3334,18 +3346,18 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -3357,15 +3369,15 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -3377,15 +3389,15 @@
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -3397,15 +3409,15 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -3417,15 +3429,15 @@
         <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -3434,18 +3446,18 @@
         <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -3454,18 +3466,18 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F47" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -3474,23 +3486,38 @@
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F48" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -3499,38 +3526,23 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>115</v>
       </c>
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
-        <v>120</v>
-      </c>
-      <c r="E51" t="s">
-        <v>153</v>
-      </c>
-      <c r="F51" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -3539,23 +3551,38 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="E52" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F52" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" t="s">
+        <v>144</v>
+      </c>
+      <c r="F53" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
@@ -3564,38 +3591,23 @@
         <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="F54" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
-      </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>123</v>
-      </c>
-      <c r="E55" t="s">
-        <v>155</v>
-      </c>
-      <c r="F55" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -3604,18 +3616,18 @@
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E56" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="F56" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -3624,40 +3636,58 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E57" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F57" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>153</v>
+      </c>
+      <c r="E58" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" t="s">
+        <v>147</v>
+      </c>
+      <c r="F59" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -3668,7 +3698,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -3679,7 +3709,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3687,83 +3717,77 @@
       <c r="C62" t="s">
         <v>11</v>
       </c>
-      <c r="G62" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" t="s">
         <v>11</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>11</v>
       </c>
-      <c r="G63" t="s">
-        <v>98</v>
+      <c r="G64" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" t="s">
-        <v>53</v>
-      </c>
-      <c r="E66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F66" t="s">
-        <v>102</v>
-      </c>
-      <c r="G66" t="s">
-        <v>125</v>
+        <v>97</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
-      </c>
-      <c r="B67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
-        <v>53</v>
-      </c>
-      <c r="E67" t="s">
-        <v>158</v>
-      </c>
-      <c r="F67" t="s">
-        <v>104</v>
-      </c>
-      <c r="G67" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" t="s">
+        <v>148</v>
+      </c>
+      <c r="F68" t="s">
+        <v>100</v>
+      </c>
+      <c r="G68" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -3772,37 +3796,65 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="E69" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="F69" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="G69" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>118</v>
+      </c>
+      <c r="E71" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" t="s">
+        <v>150</v>
+      </c>
+      <c r="F72" t="s">
         <v>107</v>
       </c>
-      <c r="B70" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>120</v>
-      </c>
-      <c r="E70" t="s">
-        <v>159</v>
-      </c>
-      <c r="F70" t="s">
-        <v>109</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G70" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
+  <autoFilter ref="A1:G72" xr:uid="{8D221ED8-92E6-4BAD-A179-F354ED49DF1B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added README tab + added meteo to functionalities
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HydroLib\docs\topics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BEA61-88B5-43B7-9038-18238630B32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8A618-B936-4728-BE07-C0C79A7A6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-195" yWindow="-195" windowWidth="29190" windowHeight="16140" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Source table" sheetId="2" r:id="rId4"/>
     <sheet name="mkdocs symbols" sheetId="3" r:id="rId5"/>
     <sheet name="Topics" sheetId="6" r:id="rId6"/>
+    <sheet name="README" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Source table'!$B$1:$K$69</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="183">
   <si>
     <t>Functionality</t>
   </si>
@@ -594,6 +595,27 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>* Only edit the visible (non-Hidden) columns. The two hidden columns automatically produce Markdown code for the table icons.</t>
+  </si>
+  <si>
+    <t>* Adding/changing entries in the functionalities list should be done only in the Source table tab sheet.</t>
+  </si>
+  <si>
+    <t>Inner workings</t>
+  </si>
+  <si>
+    <t>* The three first tab sheets automatically fill up based on the Source table and the kernel topic name (using FILTER and SELECTCOLS)</t>
+  </si>
+  <si>
+    <t>* As the Source table grows longer, make sure that on the first three tabs the select formula in A3 still includes all row numbers for which Source table has data values.</t>
+  </si>
+  <si>
+    <t>Meteo</t>
   </si>
 </sst>
 </file>
@@ -957,20 +979,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90FEF51-A5AE-374B-98FD-FAB0AC3382D4}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>Topics!A3</f>
         <v>DIMR</v>
@@ -1011,7 +1033,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="str" cm="1">
         <f t="array" ref="A3:F8">IF(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10)=0," ",_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10))</f>
         <v>`dimr_config.xml`</v>
@@ -1032,7 +1054,7 @@
         <v>Critical bugfix for [#127](https://github.com/Deltares/HYDROLIB-core/issues/127).</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <v>FM component</v>
       </c>
@@ -1052,7 +1074,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <v>RR component</v>
       </c>
@@ -1072,7 +1094,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <v>RTC component</v>
       </c>
@@ -1092,7 +1114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <v>parallel MPI models</v>
       </c>
@@ -1112,7 +1134,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <v>coupler elements</v>
       </c>
@@ -1143,19 +1165,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>Topics!A2</f>
         <v>RR</v>
@@ -1196,7 +1218,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="str" cm="1">
         <f t="array" ref="A3:F7">IF(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10)=0," ",_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10))</f>
         <v>Main sobek_3b.fnm</v>
@@ -1217,7 +1239,7 @@
         <v>Used to be in hydrolib.core.io.fnm.models before 0.3.0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <v>Rainfall .bui file</v>
       </c>
@@ -1237,7 +1259,7 @@
         <v>Used to be in hydrolib.core.io.bui.models before 0.3.0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <v>**Topology layer**</v>
       </c>
@@ -1257,7 +1279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <v>Node file 3b_node.tp</v>
       </c>
@@ -1277,7 +1299,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <v>Link file 3b_link.tp</v>
       </c>
@@ -1308,19 +1330,19 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>Topics!A1</f>
         <v>FM</v>
@@ -1361,7 +1383,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="str" cm="1">
         <f t="array" ref="A3:F57">IF(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10)=0," ",_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER('Source table'!B2:K95,'Source table'!A2:A95=A2," "),1,3,5,6,9,10))</f>
         <v>MDU file</v>
@@ -1382,7 +1404,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <v>Network file `_net.nc`</v>
       </c>
@@ -1402,7 +1424,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <v>**Structure file**</v>
       </c>
@@ -1422,7 +1444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <v>* Weir</v>
       </c>
@@ -1442,7 +1464,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <v>* Universal weir</v>
       </c>
@@ -1462,7 +1484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <v>* Culvert</v>
       </c>
@@ -1482,7 +1504,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <v>* Long culvert</v>
       </c>
@@ -1502,7 +1524,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <v>* Bridge</v>
       </c>
@@ -1522,7 +1544,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <v>* Pump</v>
       </c>
@@ -1542,7 +1564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <v>* Orifice</v>
       </c>
@@ -1562,7 +1584,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <v>* Gate</v>
       </c>
@@ -1582,7 +1604,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <v>* General structure</v>
       </c>
@@ -1602,7 +1624,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <v>* Dambreak</v>
       </c>
@@ -1622,7 +1644,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <v>* Compound structure</v>
       </c>
@@ -1642,7 +1664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <v>**External forcings file**</v>
       </c>
@@ -1662,7 +1684,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
         <v>External forcings file (old)</v>
       </c>
@@ -1682,7 +1704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <v>External forcings file (new)</v>
       </c>
@@ -1702,7 +1724,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
         <v>* Boundary</v>
       </c>
@@ -1722,7 +1744,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <v>* Lateral</v>
       </c>
@@ -1742,27 +1764,27 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <v>* Meteo</v>
       </c>
       <c r="B22" t="str">
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="C22" t="str">
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="D22" t="str">
-        <v xml:space="preserve"> </v>
+        <v>0.5.0</v>
       </c>
       <c r="E22" t="str">
-        <v xml:space="preserve"> </v>
+        <v>[Meteo][hydrolib.core.dflowfm.ext.models.Meteo]</v>
       </c>
       <c r="F22" t="str">
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <v xml:space="preserve"> .bc file</v>
       </c>
@@ -1782,7 +1804,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <v>* timeSeries</v>
       </c>
@@ -1802,7 +1824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <v>* harmonic (-Correction)</v>
       </c>
@@ -1822,7 +1844,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <v>* astronomic (-Correction)</v>
       </c>
@@ -1842,7 +1864,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <v>* t3D</v>
       </c>
@@ -1862,7 +1884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <v>* QHTable</v>
       </c>
@@ -1882,7 +1904,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <v>* constant</v>
       </c>
@@ -1902,7 +1924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
         <v>* vector quantities</v>
       </c>
@@ -1922,7 +1944,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
         <v xml:space="preserve"> .tim file</v>
       </c>
@@ -1942,7 +1964,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="str">
         <v>**Cross section files**</v>
       </c>
@@ -1962,7 +1984,7 @@
         <v>Moved to io.crosssections in 0.2.0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="str">
         <v>Cross section definition file</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="str">
         <v>* Circle</v>
       </c>
@@ -2002,7 +2024,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="str">
         <v>* Rectangle</v>
       </c>
@@ -2022,7 +2044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="str">
         <v>* Tabulated river</v>
       </c>
@@ -2042,7 +2064,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="str">
         <v>* ZW (tabulated)</v>
       </c>
@@ -2062,7 +2084,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="str">
         <v>* XYZ</v>
       </c>
@@ -2082,7 +2104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="str">
         <v>* YZ</v>
       </c>
@@ -2102,7 +2124,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="str">
         <v>Cross section location file</v>
       </c>
@@ -2122,7 +2144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="str">
         <v>1D roughness file</v>
       </c>
@@ -2142,7 +2164,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
         <v>Storage node file</v>
       </c>
@@ -2162,7 +2184,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
         <v>**Spatial data files**</v>
       </c>
@@ -2182,7 +2204,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
         <v>Initial and parameter field file</v>
       </c>
@@ -2202,7 +2224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
         <v>1D field INI files</v>
       </c>
@@ -2222,7 +2244,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
         <v>Sample file</v>
       </c>
@@ -2242,7 +2264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
         <v>**Output**</v>
       </c>
@@ -2262,7 +2284,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
         <v>Observation station file (.xyn)</v>
       </c>
@@ -2282,7 +2304,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
         <v>Observation station file (.ini)</v>
       </c>
@@ -2302,7 +2324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
         <v>Observation crosssection file (.pli)</v>
       </c>
@@ -2322,7 +2344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
         <v>Observation crosssection file (.ini)</v>
       </c>
@@ -2342,7 +2364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
         <v>History file `_his.nc`</v>
       </c>
@@ -2362,7 +2384,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="str">
         <v>Map file (old)</v>
       </c>
@@ -2382,7 +2404,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="str">
         <v>Map file (UGRID) `_map.nc`</v>
       </c>
@@ -2402,7 +2424,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="str">
         <v>Fourier input file</v>
       </c>
@@ -2422,7 +2444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="str">
         <v>Fourier output file `_fou.nc`</v>
       </c>
@@ -2442,7 +2464,7 @@
         <v>via map file reader</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="str">
         <v>Class map file</v>
       </c>
@@ -2473,24 +2495,24 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="74.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.86328125" customWidth="1"/>
+    <col min="9" max="9" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.73046875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="75.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
@@ -2519,7 +2541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2558,7 +2580,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2594,7 +2616,7 @@
         <v>[FMComponent][hydrolib.core.dimr.models.FMComponent]</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2630,7 +2652,7 @@
         <v>[RRComponent][hydrolib.core.dimr.models.RRComponent]</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2660,7 +2682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2696,7 +2718,7 @@
         <v>[Component][hydrolib.core.dimr.models.Component]</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>Topics!$A$3</f>
         <v>DIMR</v>
@@ -2732,7 +2754,7 @@
         <v>[Coupler][hydrolib.core.dimr.models.Coupler]</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D8" t="str">
         <f>IF(C8='mkdocs symbols'!$A$2,'mkdocs symbols'!$B$2,IF(C8='mkdocs symbols'!$A$3,'mkdocs symbols'!$B$3,IF(C8='mkdocs symbols'!$A$4,'mkdocs symbols'!$B$4,IF(C8='mkdocs symbols'!$A$5,'mkdocs symbols'!$B$5," "))))</f>
         <v xml:space="preserve"> </v>
@@ -2746,7 +2768,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2782,7 +2804,7 @@
         <v>[FMModel][hydrolib.core.dflowfm.mdu.models.FMModel]</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2818,7 +2840,7 @@
         <v>[Mesh2d][hydrolib.core.dflowfm.net.models.Mesh2d]</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2854,7 +2876,7 @@
         <v>[StructureModel][hydrolib.core.dflowfm.structure.models.StructureModel]</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2890,7 +2912,7 @@
         <v>[Weir][hydrolib.core.dflowfm.structure.models.Weir]</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2926,7 +2948,7 @@
         <v>[UniversalWeir][hydrolib.core.dflowfm.structure.models.UniversalWeir]</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2962,7 +2984,7 @@
         <v>[Culvert][hydrolib.core.dflowfm.structure.models.Culvert]</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -2989,7 +3011,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3025,7 +3047,7 @@
         <v>[Bridge][hydrolib.core.dflowfm.structure.models.Bridge]</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3061,7 +3083,7 @@
         <v>[Pump][hydrolib.core.dflowfm.structure.models.Pump]</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3097,7 +3119,7 @@
         <v>[Orifice][hydrolib.core.dflowfm.structure.models.Orifice]</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3124,7 +3146,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3160,7 +3182,7 @@
         <v>[GeneralStructure][hydrolib.core.dflowfm.structure.models.GeneralStructure]</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3196,7 +3218,7 @@
         <v>[Dambreak][hydrolib.core.dflowfm.structure.models.Dambreak]</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3232,7 +3254,7 @@
         <v>[Compound][hydrolib.core.dflowfm.structure.models.Compound]</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3241,7 +3263,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3277,7 +3299,7 @@
         <v>[ExtOldModel][hydrolib.core.dflowfm.extold.models.ExtOldModel]</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3313,7 +3335,7 @@
         <v>[ExtModel][hydrolib.core.dflowfm.ext.models.ExtModel]</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3349,7 +3371,7 @@
         <v>[Boundary][hydrolib.core.dflowfm.ext.models.Boundary]</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3385,7 +3407,7 @@
         <v>[Lateral][hydrolib.core.dflowfm.ext.models.Lateral]</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3394,25 +3416,34 @@
         <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="str">
         <f>IF(C28='mkdocs symbols'!$A$2,'mkdocs symbols'!$B$2,IF(C28='mkdocs symbols'!$A$3,'mkdocs symbols'!$B$3,IF(C28='mkdocs symbols'!$A$4,'mkdocs symbols'!$B$4,IF(C28='mkdocs symbols'!$A$5,'mkdocs symbols'!$B$5," "))))</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" t="str">
         <f>IF(E28='mkdocs symbols'!$A$2,'mkdocs symbols'!$B$2,IF(E28='mkdocs symbols'!$A$3,'mkdocs symbols'!$B$3,IF(E28='mkdocs symbols'!$A$4,'mkdocs symbols'!$B$4,IF(E28='mkdocs symbols'!$A$5,'mkdocs symbols'!$B$5," "))))</f>
-        <v>:material-close-box:</v>
+        <v>:white_check_mark:</v>
+      </c>
+      <c r="G28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" t="s">
+        <v>135</v>
+      </c>
+      <c r="I28" t="s">
+        <v>182</v>
       </c>
       <c r="J28" t="str">
         <f>IF(OR(ISBLANK('Source table'!H28),ISBLANK('Source table'!I28))," ","["&amp;'Source table'!I28&amp;"]["&amp;'Source table'!H28&amp;"."&amp;'Source table'!I28&amp;"]")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>[Meteo][hydrolib.core.dflowfm.ext.models.Meteo]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3448,7 +3479,7 @@
         <v>[ForcingModel][hydrolib.core.dflowfm.bc.models.ForcingModel]</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3484,7 +3515,7 @@
         <v>[TimeSeries][hydrolib.core.dflowfm.bc.models.TimeSeries]</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3520,7 +3551,7 @@
         <v>[Harmonic][hydrolib.core.dflowfm.bc.models.Harmonic]</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3556,7 +3587,7 @@
         <v>[Astronomic][hydrolib.core.dflowfm.bc.models.Astronomic]</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3592,7 +3623,7 @@
         <v>[T3D][hydrolib.core.dflowfm.bc.models.T3D]</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3628,7 +3659,7 @@
         <v>[QHTable][hydrolib.core.dflowfm.bc.models.QHTable]</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3664,7 +3695,7 @@
         <v>[Constant][hydrolib.core.dflowfm.bc.models.Constant]</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3700,7 +3731,7 @@
         <v>[VectorQuantityUnitPairs][hydrolib.core.dflowfm.bc.models.VectorQuantityUnitPairs]</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3736,7 +3767,7 @@
         <v>[TimModel][hydrolib.core.dflowfm.tim.models.TimModel]</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3766,7 +3797,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3802,7 +3833,7 @@
         <v>[CrossDefModel][hydrolib.core.dflowfm.crosssection.models.CrossDefModel]</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3838,7 +3869,7 @@
         <v>[CircleCrsDef][hydrolib.core.dflowfm.crosssection.models.CircleCrsDef]</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3874,7 +3905,7 @@
         <v>[RectangleCrsDef][hydrolib.core.dflowfm.crosssection.models.RectangleCrsDef]</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3910,7 +3941,7 @@
         <v>[ZWRiverCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWRiverCrsDef]</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3946,7 +3977,7 @@
         <v>[ZWCrsDef][hydrolib.core.dflowfm.crosssection.models.ZWCrsDef]</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -3982,7 +4013,7 @@
         <v>[XYZCrsDef][hydrolib.core.dflowfm.crosssection.models.XYZCrsDef]</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4018,7 +4049,7 @@
         <v>[YZCrsDef][hydrolib.core.dflowfm.crosssection.models.YZCrsDef]</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4054,7 +4085,7 @@
         <v>[CrossLocModel][hydrolib.core.dflowfm.crosssection.models.CrossLocModel]</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4090,7 +4121,7 @@
         <v>[FrictionModel][hydrolib.core.dflowfm.friction.models.FrictionModel]</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4126,7 +4157,7 @@
         <v>[StorageNodeModel][hydrolib.core.dflowfm.storagenode.models.StorageNodeModel]</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4147,7 +4178,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4183,7 +4214,7 @@
         <v>[IniFieldModel][hydrolib.core.dflowfm.inifield.models.IniFieldModel]</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4219,7 +4250,7 @@
         <v>[OneDFieldModel][hydrolib.core.dflowfm.onedfield.models.OneDFieldModel]</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4255,7 +4286,7 @@
         <v>[XYZModel][hydrolib.core.dflowfm.xyz.models.XYZModel]</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4276,7 +4307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4312,7 +4343,7 @@
         <v>[XYNModel][hydrolib.core.dflowm.xyn.models.XYNModel]</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4348,7 +4379,7 @@
         <v>[ObservationPointModel][hydrolib.core.dflowfm.obs.models.ObservationPointModel]</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4384,7 +4415,7 @@
         <v>[PolyFile][hydrolib.core.dflowfm.polyfile.models.PolyFile]</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4420,7 +4451,7 @@
         <v>[ObservationCrossSectionModel][hydrolib.core.dflowfm.obscrosssection.models.ObservationCrossSectionModel]</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4447,7 +4478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4474,7 +4505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4501,7 +4532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4528,7 +4559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4558,7 +4589,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="str">
         <f>Topics!$A$1</f>
         <v>FM</v>
@@ -4588,7 +4619,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D64" t="str">
         <f>IF(C64='mkdocs symbols'!$A$2,'mkdocs symbols'!$B$2,IF(C64='mkdocs symbols'!$A$3,'mkdocs symbols'!$B$3,IF(C64='mkdocs symbols'!$A$4,'mkdocs symbols'!$B$4,IF(C64='mkdocs symbols'!$A$5,'mkdocs symbols'!$B$5," "))))</f>
         <v xml:space="preserve"> </v>
@@ -4602,7 +4633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="str">
         <f>Topics!$A$2</f>
         <v>RR</v>
@@ -4641,7 +4672,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="str">
         <f>Topics!$A$2</f>
         <v>RR</v>
@@ -4680,7 +4711,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="str">
         <f>Topics!$A$2</f>
         <v>RR</v>
@@ -4701,7 +4732,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="str">
         <f>Topics!$A$2</f>
         <v>RR</v>
@@ -4737,7 +4768,7 @@
         <v>[NodeFile][hydrolib.core.rr.topology.models.NodeFile]</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="str">
         <f>Topics!$A$2</f>
         <v>RR</v>
@@ -4788,13 +4819,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4805,7 +4836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4816,7 +4847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -4827,7 +4858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -4838,7 +4869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -4863,19 +4894,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4884,4 +4915,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8412FF0C-0443-4685-B861-CDFBC73E1997}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix dflowm (no f) typo in excel sheet
</commit_message>
<xml_diff>
--- a/docs/topics/dhydro_support_hydrolib-core.xlsx
+++ b/docs/topics/dhydro_support_hydrolib-core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\HYDROLIB-core_git\docs\topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8A618-B936-4728-BE07-C0C79A7A6571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B02D37-DDA3-48B6-AEB1-613195F3349D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="-195" windowWidth="29190" windowHeight="16140" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A97F310A-419E-4629-B7E1-36C7C96E0559}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMR mkdocs table" sheetId="5" r:id="rId1"/>
@@ -522,9 +522,6 @@
     <t>0.5.0</t>
   </si>
   <si>
-    <t>hydrolib.core.dflowm.xyn.models</t>
-  </si>
-  <si>
     <t>XYNModel</t>
   </si>
   <si>
@@ -616,6 +613,9 @@
   </si>
   <si>
     <t>Meteo</t>
+  </si>
+  <si>
+    <t>hydrolib.core.dflowfm.xyn.models</t>
   </si>
 </sst>
 </file>
@@ -1018,19 +1018,19 @@
         <v>DIMR</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1203,19 +1203,19 @@
         <v>RR</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1368,19 +1368,19 @@
         <v>FM</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -2298,7 +2298,7 @@
         <v>0.5.0</v>
       </c>
       <c r="E48" t="str">
-        <v>[XYNModel][hydrolib.core.dflowm.xyn.models.XYNModel]</v>
+        <v>[XYNModel][hydrolib.core.dflowfm.xyn.models.XYNModel]</v>
       </c>
       <c r="F48" t="str">
         <v xml:space="preserve"> </v>
@@ -2494,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C09F23-468B-4C51-ACB5-C211040651DD}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2514,7 +2514,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3260,7 +3260,7 @@
         <v>FM</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
@@ -3289,10 +3289,10 @@
         <v>150</v>
       </c>
       <c r="H24" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" t="s">
         <v>157</v>
-      </c>
-      <c r="I24" t="s">
-        <v>158</v>
       </c>
       <c r="J24" t="str">
         <f>IF(OR(ISBLANK('Source table'!H24),ISBLANK('Source table'!I24))," ","["&amp;'Source table'!I24&amp;"]["&amp;'Source table'!H24&amp;"."&amp;'Source table'!I24&amp;"]")</f>
@@ -3305,7 +3305,7 @@
         <v>FM</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -3436,7 +3436,7 @@
         <v>135</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J28" t="str">
         <f>IF(OR(ISBLANK('Source table'!H28),ISBLANK('Source table'!I28))," ","["&amp;'Source table'!I28&amp;"]["&amp;'Source table'!H28&amp;"."&amp;'Source table'!I28&amp;"]")</f>
@@ -3449,7 +3449,7 @@
         <v>FM</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
@@ -3485,7 +3485,7 @@
         <v>FM</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
@@ -3521,7 +3521,7 @@
         <v>FM</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
         <v>FM</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -3593,7 +3593,7 @@
         <v>FM</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -3629,7 +3629,7 @@
         <v>FM</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
@@ -3665,7 +3665,7 @@
         <v>FM</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
@@ -3701,7 +3701,7 @@
         <v>FM</v>
       </c>
       <c r="B36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
@@ -3737,7 +3737,7 @@
         <v>FM</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
@@ -3757,10 +3757,10 @@
         <v>150</v>
       </c>
       <c r="H37" t="s">
+        <v>169</v>
+      </c>
+      <c r="I37" t="s">
         <v>170</v>
-      </c>
-      <c r="I37" t="s">
-        <v>171</v>
       </c>
       <c r="J37" t="str">
         <f>IF(OR(ISBLANK('Source table'!H37),ISBLANK('Source table'!I37))," ","["&amp;'Source table'!I37&amp;"]["&amp;'Source table'!H37&amp;"."&amp;'Source table'!I37&amp;"]")</f>
@@ -4333,14 +4333,14 @@
         <v>150</v>
       </c>
       <c r="H54" t="s">
+        <v>182</v>
+      </c>
+      <c r="I54" t="s">
         <v>151</v>
-      </c>
-      <c r="I54" t="s">
-        <v>152</v>
       </c>
       <c r="J54" t="str">
         <f>IF(OR(ISBLANK('Source table'!H54),ISBLANK('Source table'!I54))," ","["&amp;'Source table'!I54&amp;"]["&amp;'Source table'!H54&amp;"."&amp;'Source table'!I54&amp;"]")</f>
-        <v>[XYNModel][hydrolib.core.dflowm.xyn.models.XYNModel]</v>
+        <v>[XYNModel][hydrolib.core.dflowfm.xyn.models.XYNModel]</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
@@ -4385,7 +4385,7 @@
         <v>FM</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
@@ -4405,10 +4405,10 @@
         <v>150</v>
       </c>
       <c r="H56" t="s">
+        <v>154</v>
+      </c>
+      <c r="I56" t="s">
         <v>155</v>
-      </c>
-      <c r="I56" t="s">
-        <v>156</v>
       </c>
       <c r="J56" t="str">
         <f>IF(OR(ISBLANK('Source table'!H56),ISBLANK('Source table'!I56))," ","["&amp;'Source table'!I56&amp;"]["&amp;'Source table'!H56&amp;"."&amp;'Source table'!I56&amp;"]")</f>
@@ -4421,7 +4421,7 @@
         <v>FM</v>
       </c>
       <c r="B57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
         <v>10</v>
@@ -4898,12 +4898,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
@@ -4929,32 +4929,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>